<commit_message>
Update data processing script and upload files.
</commit_message>
<xml_diff>
--- a/data-master/Children_under_18_yrs_living_in_slums_households.xlsx
+++ b/data-master/Children_under_18_yrs_living_in_slums_households.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27030"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Dropbox\UID Data 2020\Uploaded content 2021\UNICEF Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unhcr365-my.sharepoint.com/personal/smit_unhcr_org/Documents/Documents/Datathon/Datathon/data-master/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{C566B019-667F-4F94-966A-625E4D91F8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
     <numFmt numFmtId="166" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1069,7 +1069,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="ESTIMATES"/>
@@ -1357,41 +1357,41 @@
   <dimension ref="A1:AJ448"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="X5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="AC9" sqref="AC9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="5" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" style="5" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" style="5" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="5" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" style="5" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="5" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" style="5" customWidth="1"/>
-    <col min="16" max="22" width="8.7109375" style="5" customWidth="1"/>
-    <col min="23" max="23" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.1796875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="9.7265625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="5" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" style="5" customWidth="1"/>
+    <col min="14" max="14" width="10.7265625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="9.81640625" style="5" customWidth="1"/>
+    <col min="16" max="22" width="8.7265625" style="5" customWidth="1"/>
+    <col min="23" max="23" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="19" style="1" customWidth="1"/>
-    <col min="26" max="33" width="7.140625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.42578125" style="68" customWidth="1"/>
-    <col min="36" max="36" width="18.85546875" style="41" customWidth="1"/>
-    <col min="37" max="16384" width="9.140625" style="1"/>
+    <col min="26" max="33" width="7.1796875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.453125" style="68" customWidth="1"/>
+    <col min="36" max="36" width="18.81640625" style="41" customWidth="1"/>
+    <col min="37" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="2" customFormat="1" ht="42" customHeight="1" thickTop="1">
+    <row r="1" spans="1:36" s="2" customFormat="1" ht="42" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" ht="23.25" customHeight="1">
+    <row r="2" spans="1:36" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" s="43" t="s">
         <v>13</v>
@@ -1547,7 +1547,7 @@
       <c r="AI2" s="46"/>
       <c r="AJ2" s="34"/>
     </row>
-    <row r="3" spans="1:36" s="2" customFormat="1" ht="12" customHeight="1" thickBot="1">
+    <row r="3" spans="1:36" s="2" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -1603,7 +1603,7 @@
       <c r="AI3" s="47"/>
       <c r="AJ3" s="35"/>
     </row>
-    <row r="4" spans="1:36" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="4" spans="1:36" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>26</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="AI4" s="52"/>
       <c r="AJ4" s="36"/>
     </row>
-    <row r="5" spans="1:36" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="5" spans="1:36" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="26" t="s">
         <v>27</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>1427786.9398785175</v>
       </c>
     </row>
-    <row r="6" spans="1:36" ht="12" customHeight="1">
+    <row r="6" spans="1:36" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="26" t="s">
         <v>27</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>4016552.0968155209</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>27</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>6044896.9260387486</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8" s="26" t="s">
         <v>28</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>1298567.7607098559</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
         <v>28</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>1647482.3352601156</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>28</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>1890035.2976923082</v>
       </c>
     </row>
-    <row r="11" spans="1:36">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A11" s="26" t="s">
         <v>28</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>2471439.3314270154</v>
       </c>
     </row>
-    <row r="12" spans="1:36">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
         <v>29</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>598763.73057399446</v>
       </c>
     </row>
-    <row r="13" spans="1:36">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>29</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>806275.23307765427</v>
       </c>
     </row>
-    <row r="14" spans="1:36">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A14" s="26" t="s">
         <v>29</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>1015655.4602090449</v>
       </c>
     </row>
-    <row r="15" spans="1:36">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A15" s="26" t="s">
         <v>29</v>
       </c>
@@ -2897,7 +2897,7 @@
         <v>1125284.6782646675</v>
       </c>
     </row>
-    <row r="16" spans="1:36">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
         <v>30</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>300644.14411247807</v>
       </c>
     </row>
-    <row r="17" spans="1:36">
+    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
         <v>30</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>286480.71947809885</v>
       </c>
     </row>
-    <row r="18" spans="1:36">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>30</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>248502.79893048128</v>
       </c>
     </row>
-    <row r="19" spans="1:36">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
         <v>31</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>2366081.9647704302</v>
       </c>
     </row>
-    <row r="20" spans="1:36">
+    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A20" s="26" t="s">
         <v>31</v>
       </c>
@@ -3467,7 +3467,7 @@
         <v>2573274.2171671763</v>
       </c>
     </row>
-    <row r="21" spans="1:36">
+    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
         <v>31</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>3343691.3326171478</v>
       </c>
     </row>
-    <row r="22" spans="1:36">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>32</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>1058440.6988675361</v>
       </c>
     </row>
-    <row r="23" spans="1:36">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A23" s="26" t="s">
         <v>32</v>
       </c>
@@ -3809,7 +3809,7 @@
         <v>1562129.6793349166</v>
       </c>
     </row>
-    <row r="24" spans="1:36">
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A24" s="26" t="s">
         <v>33</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>69204.854500951857</v>
       </c>
     </row>
-    <row r="25" spans="1:36">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
         <v>34</v>
       </c>
@@ -4037,7 +4037,7 @@
         <v>684819.53448228445</v>
       </c>
     </row>
-    <row r="26" spans="1:36">
+    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
         <v>34</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>992129.52590150584</v>
       </c>
     </row>
-    <row r="27" spans="1:36">
+    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
         <v>34</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>970262.35530144512</v>
       </c>
     </row>
-    <row r="28" spans="1:36">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
         <v>35</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>1625625.0786243279</v>
       </c>
     </row>
-    <row r="29" spans="1:36">
+    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
         <v>35</v>
       </c>
@@ -4493,7 +4493,7 @@
         <v>2873080.8153130091</v>
       </c>
     </row>
-    <row r="30" spans="1:36">
+    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A30" s="26" t="s">
         <v>36</v>
       </c>
@@ -4607,7 +4607,7 @@
         <v>7358922.5700442698</v>
       </c>
     </row>
-    <row r="31" spans="1:36">
+    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A31" s="26" t="s">
         <v>36</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>14109270.435906906</v>
       </c>
     </row>
-    <row r="32" spans="1:36">
+    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A32" s="27" t="s">
         <v>37</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>3202015.0841926639</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="13.9" customHeight="1">
+    <row r="33" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="27" t="s">
         <v>37</v>
       </c>
@@ -4949,7 +4949,7 @@
         <v>2403797.7657986768</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="13.9" customHeight="1">
+    <row r="34" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="27" t="s">
         <v>37</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>752488.64207919466</v>
       </c>
     </row>
-    <row r="35" spans="1:36" ht="13.9" customHeight="1">
+    <row r="35" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>37</v>
       </c>
@@ -5177,7 +5177,7 @@
         <v>1606390.9704011064</v>
       </c>
     </row>
-    <row r="36" spans="1:36" ht="13.9" customHeight="1">
+    <row r="36" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="27" t="s">
         <v>38</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>42469.46092268802</v>
       </c>
     </row>
-    <row r="37" spans="1:36" ht="13.9" customHeight="1">
+    <row r="37" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="27" t="s">
         <v>39</v>
       </c>
@@ -5405,7 +5405,7 @@
         <v>4200671.7145235119</v>
       </c>
     </row>
-    <row r="38" spans="1:36" ht="13.9" customHeight="1">
+    <row r="38" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="27" t="s">
         <v>39</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>4248074.2519261343</v>
       </c>
     </row>
-    <row r="39" spans="1:36" ht="13.9" customHeight="1">
+    <row r="39" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="27" t="s">
         <v>39</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>5927184.032272133</v>
       </c>
     </row>
-    <row r="40" spans="1:36" ht="13.9" customHeight="1">
+    <row r="40" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="27" t="s">
         <v>39</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>6390571.0649217349</v>
       </c>
     </row>
-    <row r="41" spans="1:36" ht="13.9" customHeight="1">
+    <row r="41" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="27" t="s">
         <v>39</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>9729152.4206934702</v>
       </c>
     </row>
-    <row r="42" spans="1:36" ht="13.9" customHeight="1">
+    <row r="42" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="27" t="s">
         <v>40</v>
       </c>
@@ -5975,7 +5975,7 @@
         <v>245464.74456109002</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="13.9" customHeight="1">
+    <row r="43" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="27" t="s">
         <v>40</v>
       </c>
@@ -6089,7 +6089,7 @@
         <v>380685.98144850106</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="13.9" customHeight="1">
+    <row r="44" spans="1:36" ht="13.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="27" t="s">
         <v>41</v>
       </c>
@@ -6203,7 +6203,7 @@
         <v>276016.44083307032</v>
       </c>
     </row>
-    <row r="45" spans="1:36">
+    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A45" s="27" t="s">
         <v>41</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>336602.89930000546</v>
       </c>
     </row>
-    <row r="46" spans="1:36">
+    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A46" s="27" t="s">
         <v>42</v>
       </c>
@@ -6431,7 +6431,7 @@
         <v>1692069.0390509146</v>
       </c>
     </row>
-    <row r="47" spans="1:36">
+    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A47" s="27" t="s">
         <v>42</v>
       </c>
@@ -6545,7 +6545,7 @@
         <v>2925445.9604244027</v>
       </c>
     </row>
-    <row r="48" spans="1:36">
+    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A48" s="27" t="s">
         <v>42</v>
       </c>
@@ -6659,7 +6659,7 @@
         <v>3401048.7050992213</v>
       </c>
     </row>
-    <row r="49" spans="1:36">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A49" s="27" t="s">
         <v>42</v>
       </c>
@@ -6773,7 +6773,7 @@
         <v>4042554.8557908088</v>
       </c>
     </row>
-    <row r="50" spans="1:36">
+    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A50" s="27" t="s">
         <v>43</v>
       </c>
@@ -6887,7 +6887,7 @@
         <v>618992.57742639026</v>
       </c>
     </row>
-    <row r="51" spans="1:36">
+    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A51" s="27" t="s">
         <v>43</v>
       </c>
@@ -7001,7 +7001,7 @@
         <v>1060368.6357095479</v>
       </c>
     </row>
-    <row r="52" spans="1:36">
+    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A52" s="27" t="s">
         <v>43</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>1182549.3741138943</v>
       </c>
     </row>
-    <row r="53" spans="1:36">
+    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A53" s="27" t="s">
         <v>44</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>2168274.5250544664</v>
       </c>
     </row>
-    <row r="54" spans="1:36">
+    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A54" s="27" t="s">
         <v>44</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>2055275.2103559873</v>
       </c>
     </row>
-    <row r="55" spans="1:36">
+    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A55" s="27" t="s">
         <v>44</v>
       </c>
@@ -7457,7 +7457,7 @@
         <v>3482203.2673832858</v>
       </c>
     </row>
-    <row r="56" spans="1:36">
+    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A56" s="27" t="s">
         <v>44</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>2949789.2781332335</v>
       </c>
     </row>
-    <row r="57" spans="1:36">
+    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A57" s="27" t="s">
         <v>45</v>
       </c>
@@ -7685,7 +7685,7 @@
         <v>109251.83635121286</v>
       </c>
     </row>
-    <row r="58" spans="1:36">
+    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A58" s="27" t="s">
         <v>45</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>136064.43712574852</v>
       </c>
     </row>
-    <row r="59" spans="1:36">
+    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A59" s="27" t="s">
         <v>45</v>
       </c>
@@ -7913,7 +7913,7 @@
         <v>85804.65406603663</v>
       </c>
     </row>
-    <row r="60" spans="1:36">
+    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A60" s="27" t="s">
         <v>46</v>
       </c>
@@ -8027,7 +8027,7 @@
         <v>526436.41232744767</v>
       </c>
     </row>
-    <row r="61" spans="1:36">
+    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A61" s="27" t="s">
         <v>46</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>725353.20395752892</v>
       </c>
     </row>
-    <row r="62" spans="1:36">
+    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A62" s="27" t="s">
         <v>46</v>
       </c>
@@ -8255,7 +8255,7 @@
         <v>801970.87050923333</v>
       </c>
     </row>
-    <row r="63" spans="1:36">
+    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A63" s="27" t="s">
         <v>46</v>
       </c>
@@ -8369,7 +8369,7 @@
         <v>794361.82404277055</v>
       </c>
     </row>
-    <row r="64" spans="1:36">
+    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A64" s="27" t="s">
         <v>46</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>815434.93583273259</v>
       </c>
     </row>
-    <row r="65" spans="1:36">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A65" s="27" t="s">
         <v>47</v>
       </c>
@@ -8597,7 +8597,7 @@
         <v>2302893.0318302386</v>
       </c>
     </row>
-    <row r="66" spans="1:36">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A66" s="27" t="s">
         <v>47</v>
       </c>
@@ -8711,7 +8711,7 @@
         <v>2624921.1498877569</v>
       </c>
     </row>
-    <row r="67" spans="1:36">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A67" s="27" t="s">
         <v>47</v>
       </c>
@@ -8825,7 +8825,7 @@
         <v>2898268.848230354</v>
       </c>
     </row>
-    <row r="68" spans="1:36">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A68" s="27" t="s">
         <v>47</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>3025366.6897419761</v>
       </c>
     </row>
-    <row r="69" spans="1:36">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A69" s="27" t="s">
         <v>47</v>
       </c>
@@ -9053,7 +9053,7 @@
         <v>2836491.8212392991</v>
       </c>
     </row>
-    <row r="70" spans="1:36">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A70" s="27" t="s">
         <v>48</v>
       </c>
@@ -9167,7 +9167,7 @@
         <v>462633.68895447836</v>
       </c>
     </row>
-    <row r="71" spans="1:36">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A71" s="27" t="s">
         <v>48</v>
       </c>
@@ -9281,7 +9281,7 @@
         <v>626115.72984215</v>
       </c>
     </row>
-    <row r="72" spans="1:36">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A72" s="27" t="s">
         <v>48</v>
       </c>
@@ -9395,7 +9395,7 @@
         <v>869740.43467814021</v>
       </c>
     </row>
-    <row r="73" spans="1:36">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A73" s="27" t="s">
         <v>48</v>
       </c>
@@ -9509,7 +9509,7 @@
         <v>857510.47755303408</v>
       </c>
     </row>
-    <row r="74" spans="1:36">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A74" s="27" t="s">
         <v>48</v>
       </c>
@@ -9623,7 +9623,7 @@
         <v>792908.50190435885</v>
       </c>
     </row>
-    <row r="75" spans="1:36">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A75" s="27" t="s">
         <v>48</v>
       </c>
@@ -9737,7 +9737,7 @@
         <v>521455.06509808503</v>
       </c>
     </row>
-    <row r="76" spans="1:36">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A76" s="27" t="s">
         <v>48</v>
       </c>
@@ -9851,7 +9851,7 @@
         <v>873759.42037735856</v>
       </c>
     </row>
-    <row r="77" spans="1:36">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A77" s="27" t="s">
         <v>49</v>
       </c>
@@ -9965,7 +9965,7 @@
         <v>1756039.0320222117</v>
       </c>
     </row>
-    <row r="78" spans="1:36">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A78" s="27" t="s">
         <v>49</v>
       </c>
@@ -10079,7 +10079,7 @@
         <v>1987909.9150857423</v>
       </c>
     </row>
-    <row r="79" spans="1:36">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A79" s="27" t="s">
         <v>49</v>
       </c>
@@ -10193,7 +10193,7 @@
         <v>1924971.2763837194</v>
       </c>
     </row>
-    <row r="80" spans="1:36">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A80" s="27" t="s">
         <v>49</v>
       </c>
@@ -10307,7 +10307,7 @@
         <v>1444290.8900127823</v>
       </c>
     </row>
-    <row r="81" spans="1:36">
+    <row r="81" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A81" s="27" t="s">
         <v>50</v>
       </c>
@@ -10421,7 +10421,7 @@
         <v>1866175.7548977304</v>
       </c>
     </row>
-    <row r="82" spans="1:36">
+    <row r="82" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A82" s="27" t="s">
         <v>51</v>
       </c>
@@ -10535,7 +10535,7 @@
         <v>2522227.1639899877</v>
       </c>
     </row>
-    <row r="83" spans="1:36">
+    <row r="83" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A83" s="27" t="s">
         <v>51</v>
       </c>
@@ -10649,7 +10649,7 @@
         <v>2632025.516989023</v>
       </c>
     </row>
-    <row r="84" spans="1:36">
+    <row r="84" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A84" s="27" t="s">
         <v>51</v>
       </c>
@@ -10763,7 +10763,7 @@
         <v>2981095.310407144</v>
       </c>
     </row>
-    <row r="85" spans="1:36">
+    <row r="85" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A85" s="27" t="s">
         <v>51</v>
       </c>
@@ -10877,7 +10877,7 @@
         <v>3791663.409582383</v>
       </c>
     </row>
-    <row r="86" spans="1:36">
+    <row r="86" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A86" s="27" t="s">
         <v>51</v>
       </c>
@@ -10991,7 +10991,7 @@
         <v>3029241.9490445857</v>
       </c>
     </row>
-    <row r="87" spans="1:36">
+    <row r="87" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A87" s="26" t="s">
         <v>52</v>
       </c>
@@ -11105,7 +11105,7 @@
         <v>102169.0158849516</v>
       </c>
     </row>
-    <row r="88" spans="1:36">
+    <row r="88" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A88" s="26" t="s">
         <v>52</v>
       </c>
@@ -11219,7 +11219,7 @@
         <v>138443.13461538462</v>
       </c>
     </row>
-    <row r="89" spans="1:36">
+    <row r="89" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A89" s="26" t="s">
         <v>52</v>
       </c>
@@ -11333,7 +11333,7 @@
         <v>186079.73396920844</v>
       </c>
     </row>
-    <row r="90" spans="1:36">
+    <row r="90" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A90" s="26" t="s">
         <v>53</v>
       </c>
@@ -11447,7 +11447,7 @@
         <v>968339.04487413354</v>
       </c>
     </row>
-    <row r="91" spans="1:36">
+    <row r="91" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A91" s="26" t="s">
         <v>53</v>
       </c>
@@ -11561,7 +11561,7 @@
         <v>1093115.638482813</v>
       </c>
     </row>
-    <row r="92" spans="1:36">
+    <row r="92" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A92" s="27" t="s">
         <v>54</v>
       </c>
@@ -11675,7 +11675,7 @@
         <v>18047764.411037266</v>
       </c>
     </row>
-    <row r="93" spans="1:36">
+    <row r="93" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A93" s="27" t="s">
         <v>54</v>
       </c>
@@ -11789,7 +11789,7 @@
         <v>19626340.624141041</v>
       </c>
     </row>
-    <row r="94" spans="1:36">
+    <row r="94" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A94" s="27" t="s">
         <v>54</v>
       </c>
@@ -11903,7 +11903,7 @@
         <v>23883122.583425958</v>
       </c>
     </row>
-    <row r="95" spans="1:36">
+    <row r="95" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A95" s="27" t="s">
         <v>54</v>
       </c>
@@ -12017,7 +12017,7 @@
         <v>23648992.658044554</v>
       </c>
     </row>
-    <row r="96" spans="1:36">
+    <row r="96" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A96" s="27" t="s">
         <v>54</v>
       </c>
@@ -12131,7 +12131,7 @@
         <v>26309096.462092575</v>
       </c>
     </row>
-    <row r="97" spans="1:36">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A97" s="27" t="s">
         <v>54</v>
       </c>
@@ -12245,7 +12245,7 @@
         <v>30160627.238253802</v>
       </c>
     </row>
-    <row r="98" spans="1:36">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A98" s="27" t="s">
         <v>55</v>
       </c>
@@ -12359,7 +12359,7 @@
         <v>362601.18366093363</v>
       </c>
     </row>
-    <row r="99" spans="1:36">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A99" s="27" t="s">
         <v>55</v>
       </c>
@@ -12473,7 +12473,7 @@
         <v>519992.85810337594</v>
       </c>
     </row>
-    <row r="100" spans="1:36">
+    <row r="100" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A100" s="27" t="s">
         <v>55</v>
       </c>
@@ -12587,7 +12587,7 @@
         <v>600539.81677838718</v>
       </c>
     </row>
-    <row r="101" spans="1:36">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A101" s="27" t="s">
         <v>55</v>
       </c>
@@ -12701,7 +12701,7 @@
         <v>473681.20218211197</v>
       </c>
     </row>
-    <row r="102" spans="1:36">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A102" s="27" t="s">
         <v>55</v>
       </c>
@@ -12815,7 +12815,7 @@
         <v>434053.28786791093</v>
       </c>
     </row>
-    <row r="103" spans="1:36" s="5" customFormat="1">
+    <row r="103" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A103" s="27" t="s">
         <v>55</v>
       </c>
@@ -12929,7 +12929,7 @@
         <v>432324.39232127095</v>
       </c>
     </row>
-    <row r="104" spans="1:36" s="5" customFormat="1">
+    <row r="104" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A104" s="27" t="s">
         <v>55</v>
       </c>
@@ -13043,7 +13043,7 @@
         <v>501833.42425032594</v>
       </c>
     </row>
-    <row r="105" spans="1:36" s="5" customFormat="1">
+    <row r="105" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A105" s="27" t="s">
         <v>56</v>
       </c>
@@ -13157,7 +13157,7 @@
         <v>33905.866024518393</v>
       </c>
     </row>
-    <row r="106" spans="1:36" s="5" customFormat="1">
+    <row r="106" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A106" s="27" t="s">
         <v>57</v>
       </c>
@@ -13271,7 +13271,7 @@
         <v>634589.6873770433</v>
       </c>
     </row>
-    <row r="107" spans="1:36" s="5" customFormat="1">
+    <row r="107" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A107" s="27" t="s">
         <v>57</v>
       </c>
@@ -13385,7 +13385,7 @@
         <v>1058697.9151074151</v>
       </c>
     </row>
-    <row r="108" spans="1:36" s="5" customFormat="1">
+    <row r="108" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A108" s="27" t="s">
         <v>57</v>
       </c>
@@ -13499,7 +13499,7 @@
         <v>1222191.78443301</v>
       </c>
     </row>
-    <row r="109" spans="1:36" s="5" customFormat="1">
+    <row r="109" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A109" s="27" t="s">
         <v>57</v>
       </c>
@@ -13613,7 +13613,7 @@
         <v>1495818.3395641469</v>
       </c>
     </row>
-    <row r="110" spans="1:36" s="5" customFormat="1">
+    <row r="110" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110" s="27" t="s">
         <v>57</v>
       </c>
@@ -13727,7 +13727,7 @@
         <v>1414554.1557387775</v>
       </c>
     </row>
-    <row r="111" spans="1:36" s="5" customFormat="1">
+    <row r="111" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111" s="27" t="s">
         <v>57</v>
       </c>
@@ -13841,7 +13841,7 @@
         <v>1733921.5275515362</v>
       </c>
     </row>
-    <row r="112" spans="1:36" s="5" customFormat="1">
+    <row r="112" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112" s="27" t="s">
         <v>57</v>
       </c>
@@ -13955,7 +13955,7 @@
         <v>1590448.3573032343</v>
       </c>
     </row>
-    <row r="113" spans="1:36" s="5" customFormat="1">
+    <row r="113" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113" s="27" t="s">
         <v>57</v>
       </c>
@@ -14069,7 +14069,7 @@
         <v>1313870.5840687</v>
       </c>
     </row>
-    <row r="114" spans="1:36" s="5" customFormat="1">
+    <row r="114" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114" s="27" t="s">
         <v>57</v>
       </c>
@@ -14183,7 +14183,7 @@
         <v>1388844.392731929</v>
       </c>
     </row>
-    <row r="115" spans="1:36" s="5" customFormat="1">
+    <row r="115" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115" s="27" t="s">
         <v>57</v>
       </c>
@@ -14297,7 +14297,7 @@
         <v>1279016.9729008065</v>
       </c>
     </row>
-    <row r="116" spans="1:36" s="5" customFormat="1">
+    <row r="116" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A116" s="27" t="s">
         <v>57</v>
       </c>
@@ -14411,7 +14411,7 @@
         <v>1336807.6479067809</v>
       </c>
     </row>
-    <row r="117" spans="1:36" s="5" customFormat="1">
+    <row r="117" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A117" s="27" t="s">
         <v>58</v>
       </c>
@@ -14525,7 +14525,7 @@
         <v>820212.03562527476</v>
       </c>
     </row>
-    <row r="118" spans="1:36" s="5" customFormat="1">
+    <row r="118" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A118" s="27" t="s">
         <v>58</v>
       </c>
@@ -14639,7 +14639,7 @@
         <v>881656.61467490636</v>
       </c>
     </row>
-    <row r="119" spans="1:36" s="5" customFormat="1">
+    <row r="119" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A119" s="27" t="s">
         <v>58</v>
       </c>
@@ -14753,7 +14753,7 @@
         <v>1010697.6968811533</v>
       </c>
     </row>
-    <row r="120" spans="1:36" s="5" customFormat="1">
+    <row r="120" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A120" s="27" t="s">
         <v>58</v>
       </c>
@@ -14867,7 +14867,7 @@
         <v>801553.35924839345</v>
       </c>
     </row>
-    <row r="121" spans="1:36" s="5" customFormat="1">
+    <row r="121" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A121" s="27" t="s">
         <v>59</v>
       </c>
@@ -14981,7 +14981,7 @@
         <v>4248434.5790659133</v>
       </c>
     </row>
-    <row r="122" spans="1:36" s="5" customFormat="1">
+    <row r="122" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A122" s="27" t="s">
         <v>60</v>
       </c>
@@ -15095,7 +15095,7 @@
         <v>738747.37753519812</v>
       </c>
     </row>
-    <row r="123" spans="1:36" s="5" customFormat="1">
+    <row r="123" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A123" s="27" t="s">
         <v>60</v>
       </c>
@@ -15209,7 +15209,7 @@
         <v>924166.00859212002</v>
       </c>
     </row>
-    <row r="124" spans="1:36" s="5" customFormat="1">
+    <row r="124" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="27" t="s">
         <v>61</v>
       </c>
@@ -15323,7 +15323,7 @@
         <v>1229443.8168592216</v>
       </c>
     </row>
-    <row r="125" spans="1:36" s="5" customFormat="1">
+    <row r="125" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="27" t="s">
         <v>61</v>
       </c>
@@ -15437,7 +15437,7 @@
         <v>1739280.4752615711</v>
       </c>
     </row>
-    <row r="126" spans="1:36" s="5" customFormat="1">
+    <row r="126" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A126" s="27" t="s">
         <v>61</v>
       </c>
@@ -15551,7 +15551,7 @@
         <v>2026748.094029851</v>
       </c>
     </row>
-    <row r="127" spans="1:36" s="5" customFormat="1">
+    <row r="127" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A127" s="27" t="s">
         <v>61</v>
       </c>
@@ -15665,7 +15665,7 @@
         <v>2898037.696381012</v>
       </c>
     </row>
-    <row r="128" spans="1:36" s="5" customFormat="1">
+    <row r="128" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A128" s="27" t="s">
         <v>61</v>
       </c>
@@ -15779,7 +15779,7 @@
         <v>2895986.91199345</v>
       </c>
     </row>
-    <row r="129" spans="1:36" s="5" customFormat="1">
+    <row r="129" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A129" s="27" t="s">
         <v>61</v>
       </c>
@@ -15893,7 +15893,7 @@
         <v>3036878.6061988184</v>
       </c>
     </row>
-    <row r="130" spans="1:36" s="5" customFormat="1">
+    <row r="130" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A130" s="27" t="s">
         <v>61</v>
       </c>
@@ -16007,7 +16007,7 @@
         <v>4057573.0403225804</v>
       </c>
     </row>
-    <row r="131" spans="1:36" s="5" customFormat="1">
+    <row r="131" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A131" s="27" t="s">
         <v>62</v>
       </c>
@@ -16121,7 +16121,7 @@
         <v>3247791.3984955247</v>
       </c>
     </row>
-    <row r="132" spans="1:36" s="5" customFormat="1">
+    <row r="132" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A132" s="27" t="s">
         <v>62</v>
       </c>
@@ -16235,7 +16235,7 @@
         <v>4247503.9762404682</v>
       </c>
     </row>
-    <row r="133" spans="1:36" s="5" customFormat="1">
+    <row r="133" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="27" t="s">
         <v>62</v>
       </c>
@@ -16349,7 +16349,7 @@
         <v>4362948.4212910533</v>
       </c>
     </row>
-    <row r="134" spans="1:36" s="5" customFormat="1">
+    <row r="134" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="27" t="s">
         <v>62</v>
       </c>
@@ -16463,7 +16463,7 @@
         <v>3680920.7470101197</v>
       </c>
     </row>
-    <row r="135" spans="1:36" s="5" customFormat="1">
+    <row r="135" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135" s="27" t="s">
         <v>62</v>
       </c>
@@ -16577,7 +16577,7 @@
         <v>4188070.0452799913</v>
       </c>
     </row>
-    <row r="136" spans="1:36" s="5" customFormat="1">
+    <row r="136" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136" s="27" t="s">
         <v>62</v>
       </c>
@@ -16691,7 +16691,7 @@
         <v>4417682.3369363807</v>
       </c>
     </row>
-    <row r="137" spans="1:36" s="5" customFormat="1">
+    <row r="137" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137" s="27" t="s">
         <v>63</v>
       </c>
@@ -16805,7 +16805,7 @@
         <v>821113.99461828219</v>
       </c>
     </row>
-    <row r="138" spans="1:36" s="5" customFormat="1">
+    <row r="138" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138" s="27" t="s">
         <v>63</v>
       </c>
@@ -16919,7 +16919,7 @@
         <v>1607720.107801185</v>
       </c>
     </row>
-    <row r="139" spans="1:36" s="5" customFormat="1">
+    <row r="139" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139" s="27" t="s">
         <v>63</v>
       </c>
@@ -17033,7 +17033,7 @@
         <v>1948786.2247443891</v>
       </c>
     </row>
-    <row r="140" spans="1:36" s="5" customFormat="1">
+    <row r="140" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140" s="27" t="s">
         <v>63</v>
       </c>
@@ -17147,7 +17147,7 @@
         <v>2334430.9837831291</v>
       </c>
     </row>
-    <row r="141" spans="1:36" s="5" customFormat="1">
+    <row r="141" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141" s="27" t="s">
         <v>64</v>
       </c>
@@ -17261,7 +17261,7 @@
         <v>483151.72386557213</v>
       </c>
     </row>
-    <row r="142" spans="1:36" s="5" customFormat="1">
+    <row r="142" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142" s="27" t="s">
         <v>64</v>
       </c>
@@ -17375,7 +17375,7 @@
         <v>648437.96748760471</v>
       </c>
     </row>
-    <row r="143" spans="1:36" s="5" customFormat="1">
+    <row r="143" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="27" t="s">
         <v>64</v>
       </c>
@@ -17489,7 +17489,7 @@
         <v>669303.28361858206</v>
       </c>
     </row>
-    <row r="144" spans="1:36" s="5" customFormat="1">
+    <row r="144" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144" s="56" t="s">
         <v>65</v>
       </c>
@@ -17531,7 +17531,7 @@
       <c r="AI144" s="54"/>
       <c r="AJ144" s="37"/>
     </row>
-    <row r="145" spans="1:36" s="5" customFormat="1">
+    <row r="145" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145" s="28" t="s">
         <v>66</v>
       </c>
@@ -17645,7 +17645,7 @@
         <v>3332565.0751366694</v>
       </c>
     </row>
-    <row r="146" spans="1:36" s="5" customFormat="1">
+    <row r="146" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A146" s="26" t="s">
         <v>67</v>
       </c>
@@ -17759,7 +17759,7 @@
         <v>12320590.569727136</v>
       </c>
     </row>
-    <row r="147" spans="1:36" s="5" customFormat="1">
+    <row r="147" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A147" s="26" t="s">
         <v>67</v>
       </c>
@@ -17873,7 +17873,7 @@
         <v>11805047.35048704</v>
       </c>
     </row>
-    <row r="148" spans="1:36" s="5" customFormat="1">
+    <row r="148" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A148" s="26" t="s">
         <v>67</v>
       </c>
@@ -17987,7 +17987,7 @@
         <v>13005090.025698854</v>
       </c>
     </row>
-    <row r="149" spans="1:36" s="5" customFormat="1">
+    <row r="149" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A149" s="26" t="s">
         <v>67</v>
       </c>
@@ -18101,7 +18101,7 @@
         <v>11610751.650487727</v>
       </c>
     </row>
-    <row r="150" spans="1:36" s="5" customFormat="1">
+    <row r="150" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A150" s="26" t="s">
         <v>67</v>
       </c>
@@ -18215,7 +18215,7 @@
         <v>13561241.74917179</v>
       </c>
     </row>
-    <row r="151" spans="1:36" s="5" customFormat="1">
+    <row r="151" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A151" s="26" t="s">
         <v>68</v>
       </c>
@@ -18329,7 +18329,7 @@
         <v>732982.21235989092</v>
       </c>
     </row>
-    <row r="152" spans="1:36" s="5" customFormat="1">
+    <row r="152" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A152" s="26" t="s">
         <v>68</v>
       </c>
@@ -18443,7 +18443,7 @@
         <v>887367.51681484329</v>
       </c>
     </row>
-    <row r="153" spans="1:36" s="5" customFormat="1">
+    <row r="153" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A153" s="26" t="s">
         <v>68</v>
       </c>
@@ -18557,7 +18557,7 @@
         <v>587275.60665797337</v>
       </c>
     </row>
-    <row r="154" spans="1:36" s="5" customFormat="1">
+    <row r="154" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A154" s="26" t="s">
         <v>68</v>
       </c>
@@ -18671,7 +18671,7 @@
         <v>596246.81395348848</v>
       </c>
     </row>
-    <row r="155" spans="1:36" s="5" customFormat="1">
+    <row r="155" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A155" s="26" t="s">
         <v>69</v>
       </c>
@@ -18785,7 +18785,7 @@
         <v>88284116.861237109</v>
       </c>
     </row>
-    <row r="156" spans="1:36" s="5" customFormat="1">
+    <row r="156" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A156" s="26" t="s">
         <v>69</v>
       </c>
@@ -18899,7 +18899,7 @@
         <v>78472334.926859885</v>
       </c>
     </row>
-    <row r="157" spans="1:36" s="5" customFormat="1">
+    <row r="157" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A157" s="26" t="s">
         <v>70</v>
       </c>
@@ -19015,7 +19015,7 @@
         <v>13176182.187767604</v>
       </c>
     </row>
-    <row r="158" spans="1:36" s="5" customFormat="1">
+    <row r="158" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A158" s="26" t="s">
         <v>70</v>
       </c>
@@ -19129,7 +19129,7 @@
         <v>9896542.5000710152</v>
       </c>
     </row>
-    <row r="159" spans="1:36" s="5" customFormat="1">
+    <row r="159" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A159" s="26" t="s">
         <v>70</v>
       </c>
@@ -19243,7 +19243,7 @@
         <v>15327149.091863062</v>
       </c>
     </row>
-    <row r="160" spans="1:36" s="5" customFormat="1">
+    <row r="160" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A160" s="26" t="s">
         <v>70</v>
       </c>
@@ -19357,7 +19357,7 @@
         <v>11278818.803500475</v>
       </c>
     </row>
-    <row r="161" spans="1:36" s="5" customFormat="1">
+    <row r="161" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A161" s="26" t="s">
         <v>71</v>
       </c>
@@ -19471,7 +19471,7 @@
         <v>788033.67972119874</v>
       </c>
     </row>
-    <row r="162" spans="1:36" s="5" customFormat="1">
+    <row r="162" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A162" s="26" t="s">
         <v>71</v>
       </c>
@@ -19585,7 +19585,7 @@
         <v>898957.05683894851</v>
       </c>
     </row>
-    <row r="163" spans="1:36" s="5" customFormat="1">
+    <row r="163" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A163" s="26" t="s">
         <v>71</v>
       </c>
@@ -19699,7 +19699,7 @@
         <v>8491948.9894030355</v>
       </c>
     </row>
-    <row r="164" spans="1:36" s="5" customFormat="1">
+    <row r="164" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A164" s="26" t="s">
         <v>71</v>
       </c>
@@ -19813,7 +19813,7 @@
         <v>1622429.7303970638</v>
       </c>
     </row>
-    <row r="165" spans="1:36" s="5" customFormat="1">
+    <row r="165" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A165" s="26" t="s">
         <v>71</v>
       </c>
@@ -19927,7 +19927,7 @@
         <v>1141829.7812177243</v>
       </c>
     </row>
-    <row r="166" spans="1:36" s="5" customFormat="1">
+    <row r="166" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A166" s="26" t="s">
         <v>72</v>
       </c>
@@ -20041,7 +20041,7 @@
         <v>2810371.2335625272</v>
       </c>
     </row>
-    <row r="167" spans="1:36" s="5" customFormat="1">
+    <row r="167" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A167" s="26" t="s">
         <v>73</v>
       </c>
@@ -20155,7 +20155,7 @@
         <v>811979.84134179505</v>
       </c>
     </row>
-    <row r="168" spans="1:36" s="5" customFormat="1">
+    <row r="168" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A168" s="26" t="s">
         <v>73</v>
       </c>
@@ -20269,7 +20269,7 @@
         <v>1097137.7321821037</v>
       </c>
     </row>
-    <row r="169" spans="1:36" s="5" customFormat="1">
+    <row r="169" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A169" s="26" t="s">
         <v>73</v>
       </c>
@@ -20383,7 +20383,7 @@
         <v>827073.64383561641</v>
       </c>
     </row>
-    <row r="170" spans="1:36" s="5" customFormat="1">
+    <row r="170" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A170" s="26" t="s">
         <v>73</v>
       </c>
@@ -20497,7 +20497,7 @@
         <v>1283364.7224026553</v>
       </c>
     </row>
-    <row r="171" spans="1:36" s="5" customFormat="1">
+    <row r="171" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A171" s="26" t="s">
         <v>74</v>
       </c>
@@ -20612,7 +20612,7 @@
         <v>18912666.955126815</v>
       </c>
     </row>
-    <row r="172" spans="1:36" s="5" customFormat="1">
+    <row r="172" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A172" s="26" t="s">
         <v>74</v>
       </c>
@@ -20726,7 +20726,7 @@
         <v>20131664.117842894</v>
       </c>
     </row>
-    <row r="173" spans="1:36" s="5" customFormat="1">
+    <row r="173" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A173" s="26" t="s">
         <v>74</v>
       </c>
@@ -20840,7 +20840,7 @@
         <v>22359519.690291673</v>
       </c>
     </row>
-    <row r="174" spans="1:36" s="5" customFormat="1">
+    <row r="174" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A174" s="26" t="s">
         <v>75</v>
       </c>
@@ -20954,7 +20954,7 @@
         <v>2641435.3802946899</v>
       </c>
     </row>
-    <row r="175" spans="1:36" s="5" customFormat="1">
+    <row r="175" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A175" s="26" t="s">
         <v>75</v>
       </c>
@@ -21068,7 +21068,7 @@
         <v>8900259.9947379306</v>
       </c>
     </row>
-    <row r="176" spans="1:36" s="5" customFormat="1">
+    <row r="176" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A176" s="26" t="s">
         <v>75</v>
       </c>
@@ -21182,7 +21182,7 @@
         <v>9287048.0696062092</v>
       </c>
     </row>
-    <row r="177" spans="1:36" s="5" customFormat="1">
+    <row r="177" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A177" s="26" t="s">
         <v>75</v>
       </c>
@@ -21296,7 +21296,7 @@
         <v>9128516.6437990516</v>
       </c>
     </row>
-    <row r="178" spans="1:36" s="5" customFormat="1">
+    <row r="178" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A178" s="27" t="s">
         <v>76</v>
       </c>
@@ -21410,7 +21410,7 @@
         <v>320757.54314279504</v>
       </c>
     </row>
-    <row r="179" spans="1:36" s="5" customFormat="1">
+    <row r="179" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A179" s="27" t="s">
         <v>76</v>
       </c>
@@ -21524,7 +21524,7 @@
         <v>288105.52137212647</v>
       </c>
     </row>
-    <row r="180" spans="1:36" s="5" customFormat="1">
+    <row r="180" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A180" s="27" t="s">
         <v>77</v>
       </c>
@@ -21638,7 +21638,7 @@
         <v>80962.254573267885</v>
       </c>
     </row>
-    <row r="181" spans="1:36" s="5" customFormat="1">
+    <row r="181" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A181" s="27" t="s">
         <v>77</v>
       </c>
@@ -21752,7 +21752,7 @@
         <v>68345.560280201549</v>
       </c>
     </row>
-    <row r="182" spans="1:36" s="5" customFormat="1">
+    <row r="182" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A182" s="27" t="s">
         <v>78</v>
       </c>
@@ -21866,7 +21866,7 @@
         <v>4580691.9700082177</v>
       </c>
     </row>
-    <row r="183" spans="1:36" s="5" customFormat="1">
+    <row r="183" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A183" s="27" t="s">
         <v>78</v>
       </c>
@@ -21980,7 +21980,7 @@
         <v>4704355.9822380114</v>
       </c>
     </row>
-    <row r="184" spans="1:36" s="5" customFormat="1">
+    <row r="184" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A184" s="27" t="s">
         <v>79</v>
       </c>
@@ -22094,7 +22094,7 @@
         <v>3053465.6489765677</v>
       </c>
     </row>
-    <row r="185" spans="1:36" s="5" customFormat="1">
+    <row r="185" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A185" s="27" t="s">
         <v>80</v>
       </c>
@@ -22208,7 +22208,7 @@
         <v>3122167.472336065</v>
       </c>
     </row>
-    <row r="186" spans="1:36" s="5" customFormat="1">
+    <row r="186" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A186" s="27" t="s">
         <v>80</v>
       </c>
@@ -22322,7 +22322,7 @@
         <v>2303013.5605355063</v>
       </c>
     </row>
-    <row r="187" spans="1:36" s="5" customFormat="1">
+    <row r="187" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A187" s="26" t="s">
         <v>81</v>
       </c>
@@ -22436,7 +22436,7 @@
         <v>2145987.3125707814</v>
       </c>
     </row>
-    <row r="188" spans="1:36" s="5" customFormat="1">
+    <row r="188" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A188" s="61" t="s">
         <v>82</v>
       </c>
@@ -22476,7 +22476,7 @@
       <c r="AI188" s="54"/>
       <c r="AJ188" s="37"/>
     </row>
-    <row r="189" spans="1:36" s="5" customFormat="1">
+    <row r="189" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A189" s="26" t="s">
         <v>83</v>
       </c>
@@ -22590,7 +22590,7 @@
         <v>2439218.2957337503</v>
       </c>
     </row>
-    <row r="190" spans="1:36" s="5" customFormat="1">
+    <row r="190" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A190" s="26" t="s">
         <v>83</v>
       </c>
@@ -22704,7 +22704,7 @@
         <v>1976082.0532136383</v>
       </c>
     </row>
-    <row r="191" spans="1:36" s="5" customFormat="1">
+    <row r="191" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A191" s="26" t="s">
         <v>84</v>
       </c>
@@ -22818,7 +22818,7 @@
         <v>3107173.4601753517</v>
       </c>
     </row>
-    <row r="192" spans="1:36" s="5" customFormat="1">
+    <row r="192" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A192" s="26" t="s">
         <v>84</v>
       </c>
@@ -22932,7 +22932,7 @@
         <v>3362702.2278704136</v>
       </c>
     </row>
-    <row r="193" spans="1:36" s="5" customFormat="1">
+    <row r="193" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A193" s="26" t="s">
         <v>84</v>
       </c>
@@ -23046,7 +23046,7 @@
         <v>5889571.8507837765</v>
       </c>
     </row>
-    <row r="194" spans="1:36" s="5" customFormat="1">
+    <row r="194" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A194" s="26" t="s">
         <v>84</v>
       </c>
@@ -23160,7 +23160,7 @@
         <v>4234673.1312148385</v>
       </c>
     </row>
-    <row r="195" spans="1:36" s="5" customFormat="1">
+    <row r="195" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A195" s="26" t="s">
         <v>85</v>
       </c>
@@ -23274,7 +23274,7 @@
         <v>1046113.6968369759</v>
       </c>
     </row>
-    <row r="196" spans="1:36" s="5" customFormat="1">
+    <row r="196" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A196" s="26" t="s">
         <v>85</v>
       </c>
@@ -23388,7 +23388,7 @@
         <v>765281.83746185806</v>
       </c>
     </row>
-    <row r="197" spans="1:36" s="5" customFormat="1">
+    <row r="197" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A197" s="26" t="s">
         <v>85</v>
       </c>
@@ -23502,7 +23502,7 @@
         <v>899983.932950521</v>
       </c>
     </row>
-    <row r="198" spans="1:36" s="5" customFormat="1">
+    <row r="198" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A198" s="27" t="s">
         <v>86</v>
       </c>
@@ -23616,7 +23616,7 @@
         <v>1681850.7880239526</v>
       </c>
     </row>
-    <row r="199" spans="1:36" s="5" customFormat="1">
+    <row r="199" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A199" s="27" t="s">
         <v>87</v>
       </c>
@@ -23730,7 +23730,7 @@
         <v>51733.359248461289</v>
       </c>
     </row>
-    <row r="200" spans="1:36" s="5" customFormat="1">
+    <row r="200" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A200" s="27" t="s">
         <v>87</v>
       </c>
@@ -23844,7 +23844,7 @@
         <v>35843.494300518134</v>
       </c>
     </row>
-    <row r="201" spans="1:36" s="5" customFormat="1">
+    <row r="201" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A201" s="26" t="s">
         <v>88</v>
       </c>
@@ -23958,7 +23958,7 @@
         <v>430262.39702510065</v>
       </c>
     </row>
-    <row r="202" spans="1:36" s="5" customFormat="1">
+    <row r="202" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A202" s="26" t="s">
         <v>88</v>
       </c>
@@ -24072,7 +24072,7 @@
         <v>1349543.6193305154</v>
       </c>
     </row>
-    <row r="203" spans="1:36" s="5" customFormat="1">
+    <row r="203" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A203" s="26" t="s">
         <v>88</v>
       </c>
@@ -24186,7 +24186,7 @@
         <v>1246415.7509704132</v>
       </c>
     </row>
-    <row r="204" spans="1:36" s="5" customFormat="1">
+    <row r="204" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A204" s="26" t="s">
         <v>88</v>
       </c>
@@ -24300,7 +24300,7 @@
         <v>1309774.0239904569</v>
       </c>
     </row>
-    <row r="205" spans="1:36" s="5" customFormat="1">
+    <row r="205" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A205" s="26" t="s">
         <v>89</v>
       </c>
@@ -24414,7 +24414,7 @@
         <v>792122.10986247018</v>
       </c>
     </row>
-    <row r="206" spans="1:36" s="5" customFormat="1">
+    <row r="206" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A206" s="26" t="s">
         <v>89</v>
       </c>
@@ -24528,7 +24528,7 @@
         <v>1245949.5840592398</v>
       </c>
     </row>
-    <row r="207" spans="1:36" s="5" customFormat="1">
+    <row r="207" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A207" s="26" t="s">
         <v>90</v>
       </c>
@@ -24642,7 +24642,7 @@
         <v>940155.11789996363</v>
       </c>
     </row>
-    <row r="208" spans="1:36" s="5" customFormat="1">
+    <row r="208" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A208" s="26" t="s">
         <v>91</v>
       </c>
@@ -24757,7 +24757,7 @@
         <v>3925767.1481568329</v>
       </c>
     </row>
-    <row r="209" spans="1:36" s="5" customFormat="1">
+    <row r="209" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A209" s="26" t="s">
         <v>91</v>
       </c>
@@ -24874,7 +24874,7 @@
         <v>3721187.3813272677</v>
       </c>
     </row>
-    <row r="210" spans="1:36" s="5" customFormat="1">
+    <row r="210" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A210" s="26" t="s">
         <v>91</v>
       </c>
@@ -24988,7 +24988,7 @@
         <v>2490438.2717626859</v>
       </c>
     </row>
-    <row r="211" spans="1:36" s="5" customFormat="1">
+    <row r="211" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A211" s="26" t="s">
         <v>91</v>
       </c>
@@ -25102,7 +25102,7 @@
         <v>2396232.8102615755</v>
       </c>
     </row>
-    <row r="212" spans="1:36" s="5" customFormat="1">
+    <row r="212" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A212" s="26" t="s">
         <v>91</v>
       </c>
@@ -25216,7 +25216,7 @@
         <v>2206617.0309583186</v>
       </c>
     </row>
-    <row r="213" spans="1:36" s="5" customFormat="1" ht="12.6" thickBot="1">
+    <row r="213" spans="1:36" s="5" customFormat="1" ht="12.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A213" s="29" t="s">
         <v>91</v>
       </c>
@@ -25331,7 +25331,7 @@
         <v>2199105.8299838365</v>
       </c>
     </row>
-    <row r="214" spans="1:36" s="5" customFormat="1">
+    <row r="214" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A214" s="4"/>
       <c r="I214" s="6"/>
       <c r="J214" s="6"/>
@@ -25348,7 +25348,7 @@
       <c r="AI214" s="66"/>
       <c r="AJ214" s="39"/>
     </row>
-    <row r="215" spans="1:36" s="5" customFormat="1">
+    <row r="215" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A215" s="4"/>
       <c r="I215" s="6"/>
       <c r="J215" s="6"/>
@@ -25365,7 +25365,7 @@
       <c r="AI215" s="67"/>
       <c r="AJ215" s="40"/>
     </row>
-    <row r="216" spans="1:36" s="5" customFormat="1">
+    <row r="216" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A216" s="14" t="s">
         <v>92</v>
       </c>
@@ -25384,7 +25384,7 @@
       <c r="AI216" s="67"/>
       <c r="AJ216" s="40"/>
     </row>
-    <row r="217" spans="1:36" s="5" customFormat="1">
+    <row r="217" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A217" s="14" t="s">
         <v>93</v>
       </c>
@@ -25403,7 +25403,7 @@
       <c r="AI217" s="67"/>
       <c r="AJ217" s="40"/>
     </row>
-    <row r="218" spans="1:36" s="5" customFormat="1">
+    <row r="218" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A218" s="14" t="s">
         <v>94</v>
       </c>
@@ -25422,7 +25422,7 @@
       <c r="AI218" s="67"/>
       <c r="AJ218" s="40"/>
     </row>
-    <row r="219" spans="1:36" s="5" customFormat="1">
+    <row r="219" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A219" s="4"/>
       <c r="I219" s="6"/>
       <c r="J219" s="6"/>
@@ -25439,7 +25439,7 @@
       <c r="AI219" s="67"/>
       <c r="AJ219" s="40"/>
     </row>
-    <row r="220" spans="1:36" s="5" customFormat="1">
+    <row r="220" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A220" s="4"/>
       <c r="I220" s="6"/>
       <c r="J220" s="6"/>
@@ -25456,7 +25456,7 @@
       <c r="AI220" s="67"/>
       <c r="AJ220" s="40"/>
     </row>
-    <row r="221" spans="1:36" s="5" customFormat="1">
+    <row r="221" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A221" s="4"/>
       <c r="I221" s="6"/>
       <c r="J221" s="6"/>
@@ -25473,7 +25473,7 @@
       <c r="AI221" s="67"/>
       <c r="AJ221" s="40"/>
     </row>
-    <row r="222" spans="1:36" s="5" customFormat="1">
+    <row r="222" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A222" s="4"/>
       <c r="I222" s="6"/>
       <c r="J222" s="6"/>
@@ -25490,7 +25490,7 @@
       <c r="AI222" s="67"/>
       <c r="AJ222" s="40"/>
     </row>
-    <row r="223" spans="1:36" s="5" customFormat="1">
+    <row r="223" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A223" s="4"/>
       <c r="I223" s="6"/>
       <c r="J223" s="6"/>
@@ -25507,7 +25507,7 @@
       <c r="AI223" s="67"/>
       <c r="AJ223" s="40"/>
     </row>
-    <row r="224" spans="1:36" s="5" customFormat="1">
+    <row r="224" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A224" s="4"/>
       <c r="I224" s="6"/>
       <c r="J224" s="6"/>
@@ -25524,7 +25524,7 @@
       <c r="AI224" s="67"/>
       <c r="AJ224" s="40"/>
     </row>
-    <row r="225" spans="1:36" s="5" customFormat="1">
+    <row r="225" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A225" s="4"/>
       <c r="I225" s="6"/>
       <c r="J225" s="6"/>
@@ -25541,7 +25541,7 @@
       <c r="AI225" s="67"/>
       <c r="AJ225" s="40"/>
     </row>
-    <row r="226" spans="1:36" s="5" customFormat="1">
+    <row r="226" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A226" s="4"/>
       <c r="I226" s="6"/>
       <c r="J226" s="6"/>
@@ -25558,7 +25558,7 @@
       <c r="AI226" s="67"/>
       <c r="AJ226" s="40"/>
     </row>
-    <row r="227" spans="1:36" s="5" customFormat="1">
+    <row r="227" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A227" s="4"/>
       <c r="I227" s="6"/>
       <c r="J227" s="6"/>
@@ -25575,7 +25575,7 @@
       <c r="AI227" s="67"/>
       <c r="AJ227" s="40"/>
     </row>
-    <row r="228" spans="1:36" s="5" customFormat="1">
+    <row r="228" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A228" s="4"/>
       <c r="I228" s="6"/>
       <c r="J228" s="6"/>
@@ -25592,7 +25592,7 @@
       <c r="AI228" s="67"/>
       <c r="AJ228" s="40"/>
     </row>
-    <row r="229" spans="1:36" s="5" customFormat="1">
+    <row r="229" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A229" s="4"/>
       <c r="I229" s="6"/>
       <c r="J229" s="6"/>
@@ -25609,7 +25609,7 @@
       <c r="AI229" s="67"/>
       <c r="AJ229" s="40"/>
     </row>
-    <row r="230" spans="1:36" s="5" customFormat="1">
+    <row r="230" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A230" s="4"/>
       <c r="I230" s="6"/>
       <c r="J230" s="6"/>
@@ -25626,7 +25626,7 @@
       <c r="AI230" s="67"/>
       <c r="AJ230" s="40"/>
     </row>
-    <row r="231" spans="1:36" s="5" customFormat="1">
+    <row r="231" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A231" s="4"/>
       <c r="I231" s="6"/>
       <c r="J231" s="6"/>
@@ -25643,7 +25643,7 @@
       <c r="AI231" s="67"/>
       <c r="AJ231" s="40"/>
     </row>
-    <row r="232" spans="1:36" s="5" customFormat="1">
+    <row r="232" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A232" s="4"/>
       <c r="I232" s="6"/>
       <c r="J232" s="6"/>
@@ -25660,7 +25660,7 @@
       <c r="AI232" s="67"/>
       <c r="AJ232" s="40"/>
     </row>
-    <row r="233" spans="1:36" s="5" customFormat="1">
+    <row r="233" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A233" s="4"/>
       <c r="I233" s="6"/>
       <c r="J233" s="6"/>
@@ -25677,7 +25677,7 @@
       <c r="AI233" s="67"/>
       <c r="AJ233" s="40"/>
     </row>
-    <row r="234" spans="1:36" s="5" customFormat="1">
+    <row r="234" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A234" s="4"/>
       <c r="I234" s="6"/>
       <c r="J234" s="6"/>
@@ -25694,7 +25694,7 @@
       <c r="AI234" s="67"/>
       <c r="AJ234" s="40"/>
     </row>
-    <row r="235" spans="1:36" s="5" customFormat="1">
+    <row r="235" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A235" s="4"/>
       <c r="I235" s="6"/>
       <c r="J235" s="6"/>
@@ -25711,7 +25711,7 @@
       <c r="AI235" s="67"/>
       <c r="AJ235" s="40"/>
     </row>
-    <row r="236" spans="1:36" s="5" customFormat="1">
+    <row r="236" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A236" s="4"/>
       <c r="I236" s="6"/>
       <c r="J236" s="6"/>
@@ -25728,7 +25728,7 @@
       <c r="AI236" s="67"/>
       <c r="AJ236" s="40"/>
     </row>
-    <row r="237" spans="1:36" s="5" customFormat="1">
+    <row r="237" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A237" s="4"/>
       <c r="I237" s="6"/>
       <c r="J237" s="6"/>
@@ -25745,7 +25745,7 @@
       <c r="AI237" s="67"/>
       <c r="AJ237" s="40"/>
     </row>
-    <row r="238" spans="1:36" s="5" customFormat="1">
+    <row r="238" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A238" s="4"/>
       <c r="I238" s="6"/>
       <c r="J238" s="6"/>
@@ -25762,7 +25762,7 @@
       <c r="AI238" s="67"/>
       <c r="AJ238" s="40"/>
     </row>
-    <row r="239" spans="1:36" s="5" customFormat="1">
+    <row r="239" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A239" s="4"/>
       <c r="I239" s="6"/>
       <c r="J239" s="6"/>
@@ -25779,7 +25779,7 @@
       <c r="AI239" s="67"/>
       <c r="AJ239" s="40"/>
     </row>
-    <row r="240" spans="1:36" s="5" customFormat="1">
+    <row r="240" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A240" s="4"/>
       <c r="I240" s="6"/>
       <c r="J240" s="6"/>
@@ -25796,7 +25796,7 @@
       <c r="AI240" s="67"/>
       <c r="AJ240" s="40"/>
     </row>
-    <row r="241" spans="1:36" s="5" customFormat="1">
+    <row r="241" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A241" s="4"/>
       <c r="I241" s="6"/>
       <c r="J241" s="6"/>
@@ -25813,7 +25813,7 @@
       <c r="AI241" s="67"/>
       <c r="AJ241" s="40"/>
     </row>
-    <row r="242" spans="1:36" s="5" customFormat="1">
+    <row r="242" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A242" s="4"/>
       <c r="I242" s="6"/>
       <c r="J242" s="6"/>
@@ -25830,7 +25830,7 @@
       <c r="AI242" s="67"/>
       <c r="AJ242" s="40"/>
     </row>
-    <row r="243" spans="1:36" s="5" customFormat="1">
+    <row r="243" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A243" s="4"/>
       <c r="I243" s="6"/>
       <c r="J243" s="6"/>
@@ -25847,7 +25847,7 @@
       <c r="AI243" s="67"/>
       <c r="AJ243" s="40"/>
     </row>
-    <row r="244" spans="1:36" s="5" customFormat="1">
+    <row r="244" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A244" s="4"/>
       <c r="I244" s="6"/>
       <c r="J244" s="6"/>
@@ -25864,7 +25864,7 @@
       <c r="AI244" s="67"/>
       <c r="AJ244" s="40"/>
     </row>
-    <row r="245" spans="1:36" s="5" customFormat="1">
+    <row r="245" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A245" s="4"/>
       <c r="I245" s="6"/>
       <c r="J245" s="6"/>
@@ -25881,7 +25881,7 @@
       <c r="AI245" s="67"/>
       <c r="AJ245" s="40"/>
     </row>
-    <row r="246" spans="1:36" s="5" customFormat="1">
+    <row r="246" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A246" s="4"/>
       <c r="I246" s="6"/>
       <c r="J246" s="6"/>
@@ -25898,7 +25898,7 @@
       <c r="AI246" s="67"/>
       <c r="AJ246" s="40"/>
     </row>
-    <row r="247" spans="1:36" s="5" customFormat="1">
+    <row r="247" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A247" s="4"/>
       <c r="I247" s="6"/>
       <c r="J247" s="6"/>
@@ -25915,7 +25915,7 @@
       <c r="AI247" s="67"/>
       <c r="AJ247" s="40"/>
     </row>
-    <row r="248" spans="1:36" s="5" customFormat="1">
+    <row r="248" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A248" s="4"/>
       <c r="I248" s="6"/>
       <c r="J248" s="6"/>
@@ -25932,7 +25932,7 @@
       <c r="AI248" s="67"/>
       <c r="AJ248" s="40"/>
     </row>
-    <row r="249" spans="1:36" s="5" customFormat="1">
+    <row r="249" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A249" s="4"/>
       <c r="I249" s="6"/>
       <c r="J249" s="6"/>
@@ -25949,7 +25949,7 @@
       <c r="AI249" s="67"/>
       <c r="AJ249" s="40"/>
     </row>
-    <row r="250" spans="1:36" s="5" customFormat="1">
+    <row r="250" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A250" s="4"/>
       <c r="I250" s="6"/>
       <c r="J250" s="6"/>
@@ -25966,7 +25966,7 @@
       <c r="AI250" s="67"/>
       <c r="AJ250" s="40"/>
     </row>
-    <row r="251" spans="1:36" s="5" customFormat="1">
+    <row r="251" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A251" s="7"/>
       <c r="I251" s="6"/>
       <c r="J251" s="6"/>
@@ -25983,7 +25983,7 @@
       <c r="AI251" s="67"/>
       <c r="AJ251" s="40"/>
     </row>
-    <row r="252" spans="1:36" s="5" customFormat="1">
+    <row r="252" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A252" s="4"/>
       <c r="I252" s="6"/>
       <c r="J252" s="6"/>
@@ -26000,7 +26000,7 @@
       <c r="AI252" s="67"/>
       <c r="AJ252" s="40"/>
     </row>
-    <row r="253" spans="1:36" s="5" customFormat="1">
+    <row r="253" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A253" s="4"/>
       <c r="I253" s="6"/>
       <c r="J253" s="6"/>
@@ -26017,7 +26017,7 @@
       <c r="AI253" s="67"/>
       <c r="AJ253" s="40"/>
     </row>
-    <row r="254" spans="1:36" s="5" customFormat="1">
+    <row r="254" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A254" s="4"/>
       <c r="I254" s="6"/>
       <c r="J254" s="6"/>
@@ -26034,7 +26034,7 @@
       <c r="AI254" s="67"/>
       <c r="AJ254" s="40"/>
     </row>
-    <row r="255" spans="1:36" s="5" customFormat="1">
+    <row r="255" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A255" s="4"/>
       <c r="I255" s="6"/>
       <c r="J255" s="6"/>
@@ -26051,7 +26051,7 @@
       <c r="AI255" s="67"/>
       <c r="AJ255" s="40"/>
     </row>
-    <row r="256" spans="1:36" s="5" customFormat="1">
+    <row r="256" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A256" s="4"/>
       <c r="I256" s="6"/>
       <c r="J256" s="6"/>
@@ -26068,7 +26068,7 @@
       <c r="AI256" s="67"/>
       <c r="AJ256" s="40"/>
     </row>
-    <row r="257" spans="1:36" s="5" customFormat="1">
+    <row r="257" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A257" s="4"/>
       <c r="I257" s="6"/>
       <c r="J257" s="6"/>
@@ -26085,7 +26085,7 @@
       <c r="AI257" s="67"/>
       <c r="AJ257" s="40"/>
     </row>
-    <row r="258" spans="1:36" s="5" customFormat="1">
+    <row r="258" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A258" s="4"/>
       <c r="I258" s="6"/>
       <c r="J258" s="6"/>
@@ -26102,7 +26102,7 @@
       <c r="AI258" s="67"/>
       <c r="AJ258" s="40"/>
     </row>
-    <row r="259" spans="1:36" s="5" customFormat="1">
+    <row r="259" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A259" s="4"/>
       <c r="I259" s="6"/>
       <c r="J259" s="6"/>
@@ -26119,7 +26119,7 @@
       <c r="AI259" s="67"/>
       <c r="AJ259" s="40"/>
     </row>
-    <row r="260" spans="1:36" s="5" customFormat="1">
+    <row r="260" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A260" s="4"/>
       <c r="I260" s="6"/>
       <c r="J260" s="6"/>
@@ -26136,7 +26136,7 @@
       <c r="AI260" s="67"/>
       <c r="AJ260" s="40"/>
     </row>
-    <row r="261" spans="1:36" s="5" customFormat="1">
+    <row r="261" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A261" s="4"/>
       <c r="I261" s="6"/>
       <c r="J261" s="6"/>
@@ -26153,7 +26153,7 @@
       <c r="AI261" s="67"/>
       <c r="AJ261" s="40"/>
     </row>
-    <row r="262" spans="1:36" s="5" customFormat="1">
+    <row r="262" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A262" s="4"/>
       <c r="I262" s="6"/>
       <c r="J262" s="6"/>
@@ -26170,7 +26170,7 @@
       <c r="AI262" s="67"/>
       <c r="AJ262" s="40"/>
     </row>
-    <row r="263" spans="1:36" s="5" customFormat="1">
+    <row r="263" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A263" s="4"/>
       <c r="I263" s="6"/>
       <c r="J263" s="6"/>
@@ -26187,7 +26187,7 @@
       <c r="AI263" s="67"/>
       <c r="AJ263" s="40"/>
     </row>
-    <row r="264" spans="1:36" s="5" customFormat="1">
+    <row r="264" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A264" s="4"/>
       <c r="I264" s="6"/>
       <c r="J264" s="6"/>
@@ -26204,7 +26204,7 @@
       <c r="AI264" s="67"/>
       <c r="AJ264" s="40"/>
     </row>
-    <row r="265" spans="1:36" s="5" customFormat="1">
+    <row r="265" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A265" s="4"/>
       <c r="I265" s="6"/>
       <c r="J265" s="6"/>
@@ -26221,7 +26221,7 @@
       <c r="AI265" s="67"/>
       <c r="AJ265" s="40"/>
     </row>
-    <row r="266" spans="1:36" s="5" customFormat="1">
+    <row r="266" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A266" s="4"/>
       <c r="I266" s="6"/>
       <c r="J266" s="6"/>
@@ -26238,7 +26238,7 @@
       <c r="AI266" s="67"/>
       <c r="AJ266" s="40"/>
     </row>
-    <row r="267" spans="1:36" s="5" customFormat="1">
+    <row r="267" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A267" s="4"/>
       <c r="I267" s="6"/>
       <c r="J267" s="6"/>
@@ -26255,7 +26255,7 @@
       <c r="AI267" s="67"/>
       <c r="AJ267" s="40"/>
     </row>
-    <row r="268" spans="1:36" s="5" customFormat="1">
+    <row r="268" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A268" s="4"/>
       <c r="I268" s="6"/>
       <c r="J268" s="6"/>
@@ -26272,7 +26272,7 @@
       <c r="AI268" s="67"/>
       <c r="AJ268" s="40"/>
     </row>
-    <row r="269" spans="1:36" s="5" customFormat="1">
+    <row r="269" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A269" s="4"/>
       <c r="I269" s="6"/>
       <c r="J269" s="6"/>
@@ -26289,7 +26289,7 @@
       <c r="AI269" s="67"/>
       <c r="AJ269" s="40"/>
     </row>
-    <row r="270" spans="1:36" s="5" customFormat="1">
+    <row r="270" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A270" s="4"/>
       <c r="I270" s="6"/>
       <c r="J270" s="6"/>
@@ -26306,7 +26306,7 @@
       <c r="AI270" s="67"/>
       <c r="AJ270" s="40"/>
     </row>
-    <row r="271" spans="1:36" s="5" customFormat="1">
+    <row r="271" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A271" s="4"/>
       <c r="I271" s="6"/>
       <c r="J271" s="6"/>
@@ -26323,7 +26323,7 @@
       <c r="AI271" s="67"/>
       <c r="AJ271" s="40"/>
     </row>
-    <row r="272" spans="1:36" s="5" customFormat="1">
+    <row r="272" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A272" s="4"/>
       <c r="I272" s="6"/>
       <c r="J272" s="6"/>
@@ -26340,7 +26340,7 @@
       <c r="AI272" s="67"/>
       <c r="AJ272" s="40"/>
     </row>
-    <row r="273" spans="1:36" s="5" customFormat="1">
+    <row r="273" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A273" s="4"/>
       <c r="I273" s="6"/>
       <c r="J273" s="6"/>
@@ -26357,7 +26357,7 @@
       <c r="AI273" s="67"/>
       <c r="AJ273" s="40"/>
     </row>
-    <row r="274" spans="1:36" s="5" customFormat="1">
+    <row r="274" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A274" s="4"/>
       <c r="I274" s="6"/>
       <c r="J274" s="6"/>
@@ -26374,7 +26374,7 @@
       <c r="AI274" s="67"/>
       <c r="AJ274" s="40"/>
     </row>
-    <row r="275" spans="1:36" s="5" customFormat="1">
+    <row r="275" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A275" s="4"/>
       <c r="I275" s="6"/>
       <c r="J275" s="6"/>
@@ -26391,7 +26391,7 @@
       <c r="AI275" s="67"/>
       <c r="AJ275" s="40"/>
     </row>
-    <row r="276" spans="1:36" s="5" customFormat="1">
+    <row r="276" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A276" s="4"/>
       <c r="I276" s="6"/>
       <c r="J276" s="6"/>
@@ -26408,7 +26408,7 @@
       <c r="AI276" s="67"/>
       <c r="AJ276" s="40"/>
     </row>
-    <row r="277" spans="1:36" s="5" customFormat="1">
+    <row r="277" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A277" s="4"/>
       <c r="I277" s="6"/>
       <c r="J277" s="6"/>
@@ -26425,7 +26425,7 @@
       <c r="AI277" s="67"/>
       <c r="AJ277" s="40"/>
     </row>
-    <row r="278" spans="1:36" s="5" customFormat="1">
+    <row r="278" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A278" s="4"/>
       <c r="I278" s="6"/>
       <c r="J278" s="6"/>
@@ -26442,7 +26442,7 @@
       <c r="AI278" s="67"/>
       <c r="AJ278" s="40"/>
     </row>
-    <row r="279" spans="1:36" s="5" customFormat="1">
+    <row r="279" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A279" s="4"/>
       <c r="I279" s="6"/>
       <c r="J279" s="6"/>
@@ -26459,7 +26459,7 @@
       <c r="AI279" s="67"/>
       <c r="AJ279" s="40"/>
     </row>
-    <row r="280" spans="1:36" s="5" customFormat="1">
+    <row r="280" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A280" s="4"/>
       <c r="I280" s="6"/>
       <c r="J280" s="6"/>
@@ -26476,7 +26476,7 @@
       <c r="AI280" s="67"/>
       <c r="AJ280" s="40"/>
     </row>
-    <row r="281" spans="1:36" s="5" customFormat="1">
+    <row r="281" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A281" s="4"/>
       <c r="I281" s="6"/>
       <c r="J281" s="6"/>
@@ -26493,7 +26493,7 @@
       <c r="AI281" s="67"/>
       <c r="AJ281" s="40"/>
     </row>
-    <row r="282" spans="1:36" s="5" customFormat="1">
+    <row r="282" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A282" s="4"/>
       <c r="I282" s="6"/>
       <c r="J282" s="6"/>
@@ -26510,7 +26510,7 @@
       <c r="AI282" s="67"/>
       <c r="AJ282" s="40"/>
     </row>
-    <row r="283" spans="1:36" s="5" customFormat="1">
+    <row r="283" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A283" s="4"/>
       <c r="I283" s="6"/>
       <c r="J283" s="6"/>
@@ -26527,7 +26527,7 @@
       <c r="AI283" s="67"/>
       <c r="AJ283" s="40"/>
     </row>
-    <row r="284" spans="1:36" s="5" customFormat="1">
+    <row r="284" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A284" s="4"/>
       <c r="I284" s="6"/>
       <c r="J284" s="6"/>
@@ -26544,7 +26544,7 @@
       <c r="AI284" s="67"/>
       <c r="AJ284" s="40"/>
     </row>
-    <row r="285" spans="1:36" s="5" customFormat="1">
+    <row r="285" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A285" s="7"/>
       <c r="I285" s="6"/>
       <c r="J285" s="6"/>
@@ -26561,7 +26561,7 @@
       <c r="AI285" s="67"/>
       <c r="AJ285" s="40"/>
     </row>
-    <row r="286" spans="1:36" s="5" customFormat="1">
+    <row r="286" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A286" s="4"/>
       <c r="I286" s="6"/>
       <c r="J286" s="6"/>
@@ -26578,7 +26578,7 @@
       <c r="AI286" s="67"/>
       <c r="AJ286" s="40"/>
     </row>
-    <row r="287" spans="1:36" s="5" customFormat="1">
+    <row r="287" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A287" s="4"/>
       <c r="I287" s="6"/>
       <c r="J287" s="6"/>
@@ -26595,7 +26595,7 @@
       <c r="AI287" s="67"/>
       <c r="AJ287" s="40"/>
     </row>
-    <row r="288" spans="1:36" s="5" customFormat="1">
+    <row r="288" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A288" s="4"/>
       <c r="I288" s="6"/>
       <c r="J288" s="6"/>
@@ -26612,7 +26612,7 @@
       <c r="AI288" s="67"/>
       <c r="AJ288" s="40"/>
     </row>
-    <row r="289" spans="1:36" s="5" customFormat="1">
+    <row r="289" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A289" s="4"/>
       <c r="I289" s="6"/>
       <c r="J289" s="6"/>
@@ -26629,7 +26629,7 @@
       <c r="AI289" s="67"/>
       <c r="AJ289" s="40"/>
     </row>
-    <row r="290" spans="1:36" s="5" customFormat="1">
+    <row r="290" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A290" s="4"/>
       <c r="I290" s="6"/>
       <c r="J290" s="6"/>
@@ -26646,7 +26646,7 @@
       <c r="AI290" s="67"/>
       <c r="AJ290" s="40"/>
     </row>
-    <row r="291" spans="1:36" s="5" customFormat="1">
+    <row r="291" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A291" s="4"/>
       <c r="I291" s="6"/>
       <c r="J291" s="6"/>
@@ -26663,7 +26663,7 @@
       <c r="AI291" s="67"/>
       <c r="AJ291" s="40"/>
     </row>
-    <row r="292" spans="1:36" s="5" customFormat="1">
+    <row r="292" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A292" s="4"/>
       <c r="I292" s="6"/>
       <c r="J292" s="6"/>
@@ -26680,7 +26680,7 @@
       <c r="AI292" s="67"/>
       <c r="AJ292" s="40"/>
     </row>
-    <row r="293" spans="1:36" s="5" customFormat="1">
+    <row r="293" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A293" s="4"/>
       <c r="I293" s="6"/>
       <c r="J293" s="6"/>
@@ -26697,7 +26697,7 @@
       <c r="AI293" s="67"/>
       <c r="AJ293" s="40"/>
     </row>
-    <row r="294" spans="1:36" s="5" customFormat="1">
+    <row r="294" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A294" s="4"/>
       <c r="I294" s="6"/>
       <c r="J294" s="6"/>
@@ -26714,7 +26714,7 @@
       <c r="AI294" s="67"/>
       <c r="AJ294" s="40"/>
     </row>
-    <row r="295" spans="1:36" s="5" customFormat="1">
+    <row r="295" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A295" s="4"/>
       <c r="I295" s="6"/>
       <c r="J295" s="6"/>
@@ -26731,7 +26731,7 @@
       <c r="AI295" s="67"/>
       <c r="AJ295" s="40"/>
     </row>
-    <row r="296" spans="1:36" s="5" customFormat="1">
+    <row r="296" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A296" s="4"/>
       <c r="I296" s="6"/>
       <c r="J296" s="6"/>
@@ -26748,7 +26748,7 @@
       <c r="AI296" s="67"/>
       <c r="AJ296" s="40"/>
     </row>
-    <row r="297" spans="1:36" s="5" customFormat="1">
+    <row r="297" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A297" s="4"/>
       <c r="I297" s="6"/>
       <c r="J297" s="6"/>
@@ -26765,7 +26765,7 @@
       <c r="AI297" s="67"/>
       <c r="AJ297" s="40"/>
     </row>
-    <row r="298" spans="1:36" s="5" customFormat="1">
+    <row r="298" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A298" s="4"/>
       <c r="I298" s="6"/>
       <c r="J298" s="6"/>
@@ -26782,7 +26782,7 @@
       <c r="AI298" s="67"/>
       <c r="AJ298" s="40"/>
     </row>
-    <row r="299" spans="1:36" s="5" customFormat="1">
+    <row r="299" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A299" s="4"/>
       <c r="I299" s="6"/>
       <c r="J299" s="6"/>
@@ -26799,7 +26799,7 @@
       <c r="AI299" s="67"/>
       <c r="AJ299" s="40"/>
     </row>
-    <row r="300" spans="1:36" s="5" customFormat="1">
+    <row r="300" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A300" s="4"/>
       <c r="I300" s="6"/>
       <c r="J300" s="6"/>
@@ -26816,7 +26816,7 @@
       <c r="AI300" s="67"/>
       <c r="AJ300" s="40"/>
     </row>
-    <row r="301" spans="1:36" s="5" customFormat="1">
+    <row r="301" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A301" s="4"/>
       <c r="I301" s="6"/>
       <c r="J301" s="6"/>
@@ -26833,7 +26833,7 @@
       <c r="AI301" s="67"/>
       <c r="AJ301" s="40"/>
     </row>
-    <row r="302" spans="1:36" s="5" customFormat="1">
+    <row r="302" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A302" s="4"/>
       <c r="I302" s="6"/>
       <c r="J302" s="6"/>
@@ -26850,7 +26850,7 @@
       <c r="AI302" s="67"/>
       <c r="AJ302" s="40"/>
     </row>
-    <row r="303" spans="1:36" s="5" customFormat="1">
+    <row r="303" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A303" s="4"/>
       <c r="I303" s="6"/>
       <c r="J303" s="6"/>
@@ -26867,7 +26867,7 @@
       <c r="AI303" s="67"/>
       <c r="AJ303" s="40"/>
     </row>
-    <row r="304" spans="1:36" s="5" customFormat="1">
+    <row r="304" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A304" s="4"/>
       <c r="I304" s="6"/>
       <c r="J304" s="6"/>
@@ -26884,7 +26884,7 @@
       <c r="AI304" s="67"/>
       <c r="AJ304" s="40"/>
     </row>
-    <row r="305" spans="1:36" s="5" customFormat="1">
+    <row r="305" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A305" s="4"/>
       <c r="I305" s="6"/>
       <c r="J305" s="6"/>
@@ -26901,7 +26901,7 @@
       <c r="AI305" s="67"/>
       <c r="AJ305" s="40"/>
     </row>
-    <row r="306" spans="1:36" s="5" customFormat="1">
+    <row r="306" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A306" s="4"/>
       <c r="I306" s="6"/>
       <c r="J306" s="6"/>
@@ -26918,7 +26918,7 @@
       <c r="AI306" s="67"/>
       <c r="AJ306" s="40"/>
     </row>
-    <row r="307" spans="1:36" s="5" customFormat="1">
+    <row r="307" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A307" s="4"/>
       <c r="I307" s="6"/>
       <c r="J307" s="6"/>
@@ -26935,7 +26935,7 @@
       <c r="AI307" s="67"/>
       <c r="AJ307" s="40"/>
     </row>
-    <row r="308" spans="1:36" s="5" customFormat="1">
+    <row r="308" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A308" s="4"/>
       <c r="I308" s="6"/>
       <c r="J308" s="6"/>
@@ -26952,7 +26952,7 @@
       <c r="AI308" s="67"/>
       <c r="AJ308" s="40"/>
     </row>
-    <row r="309" spans="1:36" s="5" customFormat="1">
+    <row r="309" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A309" s="4"/>
       <c r="I309" s="6"/>
       <c r="J309" s="6"/>
@@ -26969,7 +26969,7 @@
       <c r="AI309" s="67"/>
       <c r="AJ309" s="40"/>
     </row>
-    <row r="310" spans="1:36" s="5" customFormat="1">
+    <row r="310" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A310" s="4"/>
       <c r="I310" s="6"/>
       <c r="J310" s="6"/>
@@ -26986,7 +26986,7 @@
       <c r="AI310" s="67"/>
       <c r="AJ310" s="40"/>
     </row>
-    <row r="311" spans="1:36" s="5" customFormat="1">
+    <row r="311" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A311" s="4"/>
       <c r="I311" s="6"/>
       <c r="J311" s="6"/>
@@ -27003,7 +27003,7 @@
       <c r="AI311" s="67"/>
       <c r="AJ311" s="40"/>
     </row>
-    <row r="312" spans="1:36" s="5" customFormat="1">
+    <row r="312" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A312" s="4"/>
       <c r="I312" s="6"/>
       <c r="J312" s="6"/>
@@ -27020,7 +27020,7 @@
       <c r="AI312" s="67"/>
       <c r="AJ312" s="40"/>
     </row>
-    <row r="313" spans="1:36" s="5" customFormat="1">
+    <row r="313" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A313" s="4"/>
       <c r="I313" s="6"/>
       <c r="J313" s="6"/>
@@ -27037,7 +27037,7 @@
       <c r="AI313" s="67"/>
       <c r="AJ313" s="40"/>
     </row>
-    <row r="314" spans="1:36" s="5" customFormat="1">
+    <row r="314" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A314" s="4"/>
       <c r="I314" s="6"/>
       <c r="J314" s="6"/>
@@ -27054,7 +27054,7 @@
       <c r="AI314" s="67"/>
       <c r="AJ314" s="40"/>
     </row>
-    <row r="315" spans="1:36" s="5" customFormat="1">
+    <row r="315" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A315" s="4"/>
       <c r="I315" s="6"/>
       <c r="J315" s="6"/>
@@ -27071,7 +27071,7 @@
       <c r="AI315" s="67"/>
       <c r="AJ315" s="40"/>
     </row>
-    <row r="316" spans="1:36" s="5" customFormat="1">
+    <row r="316" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A316" s="4"/>
       <c r="I316" s="6"/>
       <c r="J316" s="6"/>
@@ -27088,7 +27088,7 @@
       <c r="AI316" s="67"/>
       <c r="AJ316" s="40"/>
     </row>
-    <row r="317" spans="1:36" s="5" customFormat="1">
+    <row r="317" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A317" s="4"/>
       <c r="I317" s="6"/>
       <c r="J317" s="6"/>
@@ -27105,7 +27105,7 @@
       <c r="AI317" s="67"/>
       <c r="AJ317" s="40"/>
     </row>
-    <row r="318" spans="1:36" s="5" customFormat="1">
+    <row r="318" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A318" s="4"/>
       <c r="I318" s="6"/>
       <c r="J318" s="6"/>
@@ -27122,7 +27122,7 @@
       <c r="AI318" s="67"/>
       <c r="AJ318" s="40"/>
     </row>
-    <row r="319" spans="1:36" s="5" customFormat="1">
+    <row r="319" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A319" s="4"/>
       <c r="I319" s="6"/>
       <c r="J319" s="6"/>
@@ -27139,7 +27139,7 @@
       <c r="AI319" s="67"/>
       <c r="AJ319" s="40"/>
     </row>
-    <row r="320" spans="1:36" s="5" customFormat="1">
+    <row r="320" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A320" s="4"/>
       <c r="I320" s="6"/>
       <c r="J320" s="6"/>
@@ -27156,7 +27156,7 @@
       <c r="AI320" s="67"/>
       <c r="AJ320" s="40"/>
     </row>
-    <row r="321" spans="1:36" s="5" customFormat="1">
+    <row r="321" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A321" s="4"/>
       <c r="I321" s="6"/>
       <c r="J321" s="6"/>
@@ -27173,7 +27173,7 @@
       <c r="AI321" s="67"/>
       <c r="AJ321" s="40"/>
     </row>
-    <row r="322" spans="1:36" s="5" customFormat="1">
+    <row r="322" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A322" s="4"/>
       <c r="I322" s="6"/>
       <c r="J322" s="6"/>
@@ -27190,7 +27190,7 @@
       <c r="AI322" s="67"/>
       <c r="AJ322" s="40"/>
     </row>
-    <row r="323" spans="1:36" s="5" customFormat="1">
+    <row r="323" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A323" s="4"/>
       <c r="I323" s="6"/>
       <c r="J323" s="6"/>
@@ -27207,7 +27207,7 @@
       <c r="AI323" s="67"/>
       <c r="AJ323" s="40"/>
     </row>
-    <row r="324" spans="1:36" s="5" customFormat="1">
+    <row r="324" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A324" s="4"/>
       <c r="I324" s="6"/>
       <c r="J324" s="6"/>
@@ -27224,7 +27224,7 @@
       <c r="AI324" s="67"/>
       <c r="AJ324" s="40"/>
     </row>
-    <row r="325" spans="1:36" s="5" customFormat="1">
+    <row r="325" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A325" s="4"/>
       <c r="I325" s="6"/>
       <c r="J325" s="6"/>
@@ -27241,7 +27241,7 @@
       <c r="AI325" s="67"/>
       <c r="AJ325" s="40"/>
     </row>
-    <row r="326" spans="1:36" s="5" customFormat="1">
+    <row r="326" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A326" s="4"/>
       <c r="I326" s="6"/>
       <c r="J326" s="6"/>
@@ -27258,7 +27258,7 @@
       <c r="AI326" s="67"/>
       <c r="AJ326" s="40"/>
     </row>
-    <row r="327" spans="1:36" s="5" customFormat="1">
+    <row r="327" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A327" s="4"/>
       <c r="I327" s="6"/>
       <c r="J327" s="6"/>
@@ -27275,7 +27275,7 @@
       <c r="AI327" s="67"/>
       <c r="AJ327" s="40"/>
     </row>
-    <row r="328" spans="1:36" s="5" customFormat="1">
+    <row r="328" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A328" s="4"/>
       <c r="I328" s="6"/>
       <c r="J328" s="6"/>
@@ -27292,7 +27292,7 @@
       <c r="AI328" s="67"/>
       <c r="AJ328" s="40"/>
     </row>
-    <row r="329" spans="1:36" s="5" customFormat="1">
+    <row r="329" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A329" s="4"/>
       <c r="I329" s="6"/>
       <c r="J329" s="6"/>
@@ -27309,7 +27309,7 @@
       <c r="AI329" s="67"/>
       <c r="AJ329" s="40"/>
     </row>
-    <row r="330" spans="1:36" s="5" customFormat="1">
+    <row r="330" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A330" s="4"/>
       <c r="I330" s="6"/>
       <c r="J330" s="6"/>
@@ -27326,7 +27326,7 @@
       <c r="AI330" s="67"/>
       <c r="AJ330" s="40"/>
     </row>
-    <row r="331" spans="1:36" s="5" customFormat="1">
+    <row r="331" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A331" s="4"/>
       <c r="I331" s="6"/>
       <c r="J331" s="6"/>
@@ -27343,7 +27343,7 @@
       <c r="AI331" s="67"/>
       <c r="AJ331" s="40"/>
     </row>
-    <row r="332" spans="1:36" s="5" customFormat="1">
+    <row r="332" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A332" s="4"/>
       <c r="I332" s="6"/>
       <c r="J332" s="6"/>
@@ -27360,7 +27360,7 @@
       <c r="AI332" s="67"/>
       <c r="AJ332" s="40"/>
     </row>
-    <row r="333" spans="1:36" s="5" customFormat="1">
+    <row r="333" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A333" s="4"/>
       <c r="I333" s="6"/>
       <c r="J333" s="6"/>
@@ -27377,7 +27377,7 @@
       <c r="AI333" s="67"/>
       <c r="AJ333" s="40"/>
     </row>
-    <row r="334" spans="1:36" s="5" customFormat="1">
+    <row r="334" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A334" s="4"/>
       <c r="I334" s="6"/>
       <c r="J334" s="6"/>
@@ -27394,7 +27394,7 @@
       <c r="AI334" s="67"/>
       <c r="AJ334" s="40"/>
     </row>
-    <row r="335" spans="1:36" s="5" customFormat="1">
+    <row r="335" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A335" s="4"/>
       <c r="I335" s="6"/>
       <c r="J335" s="6"/>
@@ -27411,7 +27411,7 @@
       <c r="AI335" s="67"/>
       <c r="AJ335" s="40"/>
     </row>
-    <row r="336" spans="1:36" s="5" customFormat="1">
+    <row r="336" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A336" s="4"/>
       <c r="I336" s="6"/>
       <c r="J336" s="6"/>
@@ -27428,7 +27428,7 @@
       <c r="AI336" s="67"/>
       <c r="AJ336" s="40"/>
     </row>
-    <row r="337" spans="1:36" s="5" customFormat="1">
+    <row r="337" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A337" s="4"/>
       <c r="I337" s="6"/>
       <c r="J337" s="6"/>
@@ -27445,7 +27445,7 @@
       <c r="AI337" s="67"/>
       <c r="AJ337" s="40"/>
     </row>
-    <row r="338" spans="1:36" s="5" customFormat="1">
+    <row r="338" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A338" s="4"/>
       <c r="I338" s="6"/>
       <c r="J338" s="6"/>
@@ -27462,7 +27462,7 @@
       <c r="AI338" s="67"/>
       <c r="AJ338" s="40"/>
     </row>
-    <row r="339" spans="1:36" s="5" customFormat="1">
+    <row r="339" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A339" s="4"/>
       <c r="I339" s="6"/>
       <c r="J339" s="6"/>
@@ -27479,7 +27479,7 @@
       <c r="AI339" s="67"/>
       <c r="AJ339" s="40"/>
     </row>
-    <row r="340" spans="1:36" s="5" customFormat="1">
+    <row r="340" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A340" s="4"/>
       <c r="I340" s="6"/>
       <c r="J340" s="6"/>
@@ -27496,7 +27496,7 @@
       <c r="AI340" s="67"/>
       <c r="AJ340" s="40"/>
     </row>
-    <row r="341" spans="1:36" s="5" customFormat="1">
+    <row r="341" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A341" s="4"/>
       <c r="I341" s="6"/>
       <c r="J341" s="6"/>
@@ -27513,7 +27513,7 @@
       <c r="AI341" s="67"/>
       <c r="AJ341" s="40"/>
     </row>
-    <row r="342" spans="1:36" s="5" customFormat="1">
+    <row r="342" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A342" s="4"/>
       <c r="I342" s="6"/>
       <c r="J342" s="6"/>
@@ -27530,7 +27530,7 @@
       <c r="AI342" s="67"/>
       <c r="AJ342" s="40"/>
     </row>
-    <row r="343" spans="1:36" s="5" customFormat="1">
+    <row r="343" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A343" s="4"/>
       <c r="I343" s="6"/>
       <c r="J343" s="6"/>
@@ -27547,7 +27547,7 @@
       <c r="AI343" s="67"/>
       <c r="AJ343" s="40"/>
     </row>
-    <row r="344" spans="1:36" s="5" customFormat="1">
+    <row r="344" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A344" s="4"/>
       <c r="I344" s="6"/>
       <c r="J344" s="6"/>
@@ -27564,7 +27564,7 @@
       <c r="AI344" s="67"/>
       <c r="AJ344" s="40"/>
     </row>
-    <row r="345" spans="1:36" s="5" customFormat="1">
+    <row r="345" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A345" s="4"/>
       <c r="I345" s="6"/>
       <c r="J345" s="6"/>
@@ -27581,7 +27581,7 @@
       <c r="AI345" s="67"/>
       <c r="AJ345" s="40"/>
     </row>
-    <row r="346" spans="1:36" s="5" customFormat="1">
+    <row r="346" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A346" s="4"/>
       <c r="I346" s="6"/>
       <c r="J346" s="6"/>
@@ -27598,7 +27598,7 @@
       <c r="AI346" s="67"/>
       <c r="AJ346" s="40"/>
     </row>
-    <row r="347" spans="1:36" s="5" customFormat="1">
+    <row r="347" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A347" s="4"/>
       <c r="I347" s="6"/>
       <c r="J347" s="6"/>
@@ -27615,7 +27615,7 @@
       <c r="AI347" s="67"/>
       <c r="AJ347" s="40"/>
     </row>
-    <row r="348" spans="1:36" s="5" customFormat="1">
+    <row r="348" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A348" s="4"/>
       <c r="I348" s="6"/>
       <c r="J348" s="6"/>
@@ -27632,7 +27632,7 @@
       <c r="AI348" s="67"/>
       <c r="AJ348" s="40"/>
     </row>
-    <row r="349" spans="1:36" s="5" customFormat="1">
+    <row r="349" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A349" s="4"/>
       <c r="I349" s="6"/>
       <c r="J349" s="6"/>
@@ -27649,7 +27649,7 @@
       <c r="AI349" s="67"/>
       <c r="AJ349" s="40"/>
     </row>
-    <row r="350" spans="1:36" s="5" customFormat="1">
+    <row r="350" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A350" s="4"/>
       <c r="I350" s="6"/>
       <c r="J350" s="6"/>
@@ -27666,7 +27666,7 @@
       <c r="AI350" s="67"/>
       <c r="AJ350" s="40"/>
     </row>
-    <row r="351" spans="1:36" s="5" customFormat="1">
+    <row r="351" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A351" s="4"/>
       <c r="I351" s="6"/>
       <c r="J351" s="6"/>
@@ -27683,7 +27683,7 @@
       <c r="AI351" s="67"/>
       <c r="AJ351" s="40"/>
     </row>
-    <row r="352" spans="1:36" s="5" customFormat="1">
+    <row r="352" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A352" s="4"/>
       <c r="I352" s="6"/>
       <c r="J352" s="6"/>
@@ -27700,7 +27700,7 @@
       <c r="AI352" s="67"/>
       <c r="AJ352" s="40"/>
     </row>
-    <row r="353" spans="1:36" s="5" customFormat="1">
+    <row r="353" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A353" s="4"/>
       <c r="I353" s="6"/>
       <c r="J353" s="6"/>
@@ -27717,7 +27717,7 @@
       <c r="AI353" s="67"/>
       <c r="AJ353" s="40"/>
     </row>
-    <row r="354" spans="1:36" s="5" customFormat="1">
+    <row r="354" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A354" s="4"/>
       <c r="I354" s="6"/>
       <c r="J354" s="6"/>
@@ -27734,7 +27734,7 @@
       <c r="AI354" s="67"/>
       <c r="AJ354" s="40"/>
     </row>
-    <row r="355" spans="1:36" s="5" customFormat="1">
+    <row r="355" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A355" s="4"/>
       <c r="I355" s="6"/>
       <c r="J355" s="6"/>
@@ -27751,7 +27751,7 @@
       <c r="AI355" s="67"/>
       <c r="AJ355" s="40"/>
     </row>
-    <row r="356" spans="1:36" s="5" customFormat="1">
+    <row r="356" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A356" s="4"/>
       <c r="I356" s="6"/>
       <c r="J356" s="6"/>
@@ -27768,7 +27768,7 @@
       <c r="AI356" s="67"/>
       <c r="AJ356" s="40"/>
     </row>
-    <row r="357" spans="1:36" s="5" customFormat="1">
+    <row r="357" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A357" s="4"/>
       <c r="I357" s="6"/>
       <c r="J357" s="6"/>
@@ -27785,7 +27785,7 @@
       <c r="AI357" s="67"/>
       <c r="AJ357" s="40"/>
     </row>
-    <row r="358" spans="1:36" s="5" customFormat="1">
+    <row r="358" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A358" s="4"/>
       <c r="I358" s="6"/>
       <c r="J358" s="6"/>
@@ -27802,7 +27802,7 @@
       <c r="AI358" s="67"/>
       <c r="AJ358" s="40"/>
     </row>
-    <row r="359" spans="1:36" s="5" customFormat="1">
+    <row r="359" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A359" s="4"/>
       <c r="I359" s="6"/>
       <c r="J359" s="6"/>
@@ -27819,7 +27819,7 @@
       <c r="AI359" s="67"/>
       <c r="AJ359" s="40"/>
     </row>
-    <row r="360" spans="1:36" s="5" customFormat="1">
+    <row r="360" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A360" s="4"/>
       <c r="I360" s="6"/>
       <c r="J360" s="6"/>
@@ -27836,7 +27836,7 @@
       <c r="AI360" s="67"/>
       <c r="AJ360" s="40"/>
     </row>
-    <row r="361" spans="1:36" s="5" customFormat="1">
+    <row r="361" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A361" s="4"/>
       <c r="I361" s="6"/>
       <c r="J361" s="6"/>
@@ -27853,7 +27853,7 @@
       <c r="AI361" s="67"/>
       <c r="AJ361" s="40"/>
     </row>
-    <row r="362" spans="1:36" s="5" customFormat="1">
+    <row r="362" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A362" s="4"/>
       <c r="I362" s="6"/>
       <c r="J362" s="6"/>
@@ -27870,7 +27870,7 @@
       <c r="AI362" s="67"/>
       <c r="AJ362" s="40"/>
     </row>
-    <row r="363" spans="1:36" s="5" customFormat="1">
+    <row r="363" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A363" s="4"/>
       <c r="I363" s="6"/>
       <c r="J363" s="6"/>
@@ -27887,7 +27887,7 @@
       <c r="AI363" s="67"/>
       <c r="AJ363" s="40"/>
     </row>
-    <row r="364" spans="1:36" s="5" customFormat="1">
+    <row r="364" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A364" s="4"/>
       <c r="I364" s="6"/>
       <c r="J364" s="6"/>
@@ -27904,7 +27904,7 @@
       <c r="AI364" s="67"/>
       <c r="AJ364" s="40"/>
     </row>
-    <row r="365" spans="1:36" s="5" customFormat="1">
+    <row r="365" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A365" s="4"/>
       <c r="I365" s="6"/>
       <c r="J365" s="6"/>
@@ -27921,7 +27921,7 @@
       <c r="AI365" s="67"/>
       <c r="AJ365" s="40"/>
     </row>
-    <row r="366" spans="1:36" s="5" customFormat="1">
+    <row r="366" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A366" s="4"/>
       <c r="I366" s="6"/>
       <c r="J366" s="6"/>
@@ -27938,7 +27938,7 @@
       <c r="AI366" s="67"/>
       <c r="AJ366" s="40"/>
     </row>
-    <row r="367" spans="1:36" s="5" customFormat="1">
+    <row r="367" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A367" s="4"/>
       <c r="I367" s="6"/>
       <c r="J367" s="6"/>
@@ -27955,7 +27955,7 @@
       <c r="AI367" s="67"/>
       <c r="AJ367" s="40"/>
     </row>
-    <row r="368" spans="1:36" s="5" customFormat="1">
+    <row r="368" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A368" s="4"/>
       <c r="I368" s="6"/>
       <c r="J368" s="6"/>
@@ -27972,7 +27972,7 @@
       <c r="AI368" s="67"/>
       <c r="AJ368" s="40"/>
     </row>
-    <row r="369" spans="1:36" s="5" customFormat="1">
+    <row r="369" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A369" s="4"/>
       <c r="I369" s="6"/>
       <c r="J369" s="6"/>
@@ -27989,7 +27989,7 @@
       <c r="AI369" s="67"/>
       <c r="AJ369" s="40"/>
     </row>
-    <row r="370" spans="1:36" s="5" customFormat="1">
+    <row r="370" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A370" s="4"/>
       <c r="I370" s="6"/>
       <c r="J370" s="6"/>
@@ -28006,7 +28006,7 @@
       <c r="AI370" s="67"/>
       <c r="AJ370" s="40"/>
     </row>
-    <row r="371" spans="1:36" s="5" customFormat="1">
+    <row r="371" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A371" s="4"/>
       <c r="I371" s="6"/>
       <c r="J371" s="6"/>
@@ -28023,7 +28023,7 @@
       <c r="AI371" s="67"/>
       <c r="AJ371" s="40"/>
     </row>
-    <row r="372" spans="1:36" s="5" customFormat="1">
+    <row r="372" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A372" s="4"/>
       <c r="I372" s="6"/>
       <c r="J372" s="6"/>
@@ -28040,7 +28040,7 @@
       <c r="AI372" s="67"/>
       <c r="AJ372" s="40"/>
     </row>
-    <row r="373" spans="1:36" s="5" customFormat="1">
+    <row r="373" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A373" s="4"/>
       <c r="I373" s="6"/>
       <c r="J373" s="6"/>
@@ -28057,7 +28057,7 @@
       <c r="AI373" s="67"/>
       <c r="AJ373" s="40"/>
     </row>
-    <row r="374" spans="1:36" s="5" customFormat="1">
+    <row r="374" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A374" s="4"/>
       <c r="I374" s="6"/>
       <c r="J374" s="6"/>
@@ -28074,7 +28074,7 @@
       <c r="AI374" s="67"/>
       <c r="AJ374" s="40"/>
     </row>
-    <row r="375" spans="1:36" s="5" customFormat="1">
+    <row r="375" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A375" s="4"/>
       <c r="I375" s="6"/>
       <c r="J375" s="6"/>
@@ -28091,7 +28091,7 @@
       <c r="AI375" s="67"/>
       <c r="AJ375" s="40"/>
     </row>
-    <row r="376" spans="1:36" s="5" customFormat="1">
+    <row r="376" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A376" s="4"/>
       <c r="I376" s="6"/>
       <c r="J376" s="6"/>
@@ -28108,7 +28108,7 @@
       <c r="AI376" s="67"/>
       <c r="AJ376" s="40"/>
     </row>
-    <row r="377" spans="1:36" s="5" customFormat="1">
+    <row r="377" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A377" s="4"/>
       <c r="I377" s="6"/>
       <c r="J377" s="6"/>
@@ -28125,7 +28125,7 @@
       <c r="AI377" s="67"/>
       <c r="AJ377" s="40"/>
     </row>
-    <row r="378" spans="1:36" s="5" customFormat="1">
+    <row r="378" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A378" s="4"/>
       <c r="I378" s="6"/>
       <c r="J378" s="6"/>
@@ -28142,7 +28142,7 @@
       <c r="AI378" s="67"/>
       <c r="AJ378" s="40"/>
     </row>
-    <row r="379" spans="1:36" s="5" customFormat="1">
+    <row r="379" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A379" s="4"/>
       <c r="I379" s="6"/>
       <c r="J379" s="6"/>
@@ -28159,7 +28159,7 @@
       <c r="AI379" s="67"/>
       <c r="AJ379" s="40"/>
     </row>
-    <row r="380" spans="1:36" s="5" customFormat="1">
+    <row r="380" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A380" s="4"/>
       <c r="I380" s="6"/>
       <c r="J380" s="6"/>
@@ -28176,7 +28176,7 @@
       <c r="AI380" s="67"/>
       <c r="AJ380" s="40"/>
     </row>
-    <row r="381" spans="1:36" s="5" customFormat="1">
+    <row r="381" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A381" s="4"/>
       <c r="I381" s="6"/>
       <c r="J381" s="6"/>
@@ -28193,7 +28193,7 @@
       <c r="AI381" s="67"/>
       <c r="AJ381" s="40"/>
     </row>
-    <row r="382" spans="1:36" s="5" customFormat="1">
+    <row r="382" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A382" s="4"/>
       <c r="I382" s="6"/>
       <c r="J382" s="6"/>
@@ -28210,7 +28210,7 @@
       <c r="AI382" s="67"/>
       <c r="AJ382" s="40"/>
     </row>
-    <row r="383" spans="1:36" s="5" customFormat="1">
+    <row r="383" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A383" s="4"/>
       <c r="I383" s="6"/>
       <c r="J383" s="6"/>
@@ -28227,7 +28227,7 @@
       <c r="AI383" s="67"/>
       <c r="AJ383" s="40"/>
     </row>
-    <row r="384" spans="1:36" s="5" customFormat="1">
+    <row r="384" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A384" s="4"/>
       <c r="I384" s="6"/>
       <c r="J384" s="6"/>
@@ -28244,7 +28244,7 @@
       <c r="AI384" s="67"/>
       <c r="AJ384" s="40"/>
     </row>
-    <row r="385" spans="1:36" s="5" customFormat="1">
+    <row r="385" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A385" s="4"/>
       <c r="I385" s="6"/>
       <c r="J385" s="6"/>
@@ -28261,7 +28261,7 @@
       <c r="AI385" s="67"/>
       <c r="AJ385" s="40"/>
     </row>
-    <row r="386" spans="1:36" s="5" customFormat="1">
+    <row r="386" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A386" s="4"/>
       <c r="I386" s="6"/>
       <c r="J386" s="6"/>
@@ -28278,7 +28278,7 @@
       <c r="AI386" s="67"/>
       <c r="AJ386" s="40"/>
     </row>
-    <row r="387" spans="1:36" s="5" customFormat="1">
+    <row r="387" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A387" s="4"/>
       <c r="I387" s="6"/>
       <c r="J387" s="6"/>
@@ -28295,7 +28295,7 @@
       <c r="AI387" s="67"/>
       <c r="AJ387" s="40"/>
     </row>
-    <row r="388" spans="1:36" s="5" customFormat="1">
+    <row r="388" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A388" s="4"/>
       <c r="I388" s="6"/>
       <c r="J388" s="6"/>
@@ -28312,7 +28312,7 @@
       <c r="AI388" s="67"/>
       <c r="AJ388" s="40"/>
     </row>
-    <row r="389" spans="1:36" s="5" customFormat="1">
+    <row r="389" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A389" s="4"/>
       <c r="I389" s="6"/>
       <c r="J389" s="6"/>
@@ -28329,7 +28329,7 @@
       <c r="AI389" s="67"/>
       <c r="AJ389" s="40"/>
     </row>
-    <row r="390" spans="1:36" s="5" customFormat="1">
+    <row r="390" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A390" s="4"/>
       <c r="I390" s="6"/>
       <c r="J390" s="6"/>
@@ -28346,7 +28346,7 @@
       <c r="AI390" s="67"/>
       <c r="AJ390" s="40"/>
     </row>
-    <row r="391" spans="1:36" s="5" customFormat="1">
+    <row r="391" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A391" s="4"/>
       <c r="I391" s="6"/>
       <c r="J391" s="6"/>
@@ -28363,7 +28363,7 @@
       <c r="AI391" s="67"/>
       <c r="AJ391" s="40"/>
     </row>
-    <row r="392" spans="1:36" s="5" customFormat="1">
+    <row r="392" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A392" s="4"/>
       <c r="I392" s="6"/>
       <c r="J392" s="6"/>
@@ -28380,7 +28380,7 @@
       <c r="AI392" s="67"/>
       <c r="AJ392" s="40"/>
     </row>
-    <row r="393" spans="1:36" s="5" customFormat="1">
+    <row r="393" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A393" s="4"/>
       <c r="I393" s="6"/>
       <c r="J393" s="6"/>
@@ -28397,7 +28397,7 @@
       <c r="AI393" s="67"/>
       <c r="AJ393" s="40"/>
     </row>
-    <row r="394" spans="1:36" s="5" customFormat="1">
+    <row r="394" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A394" s="4"/>
       <c r="I394" s="6"/>
       <c r="J394" s="6"/>
@@ -28414,7 +28414,7 @@
       <c r="AI394" s="67"/>
       <c r="AJ394" s="40"/>
     </row>
-    <row r="395" spans="1:36" s="5" customFormat="1">
+    <row r="395" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A395" s="4"/>
       <c r="I395" s="6"/>
       <c r="J395" s="6"/>
@@ -28431,7 +28431,7 @@
       <c r="AI395" s="67"/>
       <c r="AJ395" s="40"/>
     </row>
-    <row r="396" spans="1:36" s="5" customFormat="1">
+    <row r="396" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A396" s="4"/>
       <c r="I396" s="6"/>
       <c r="J396" s="6"/>
@@ -28448,7 +28448,7 @@
       <c r="AI396" s="67"/>
       <c r="AJ396" s="40"/>
     </row>
-    <row r="397" spans="1:36" s="5" customFormat="1">
+    <row r="397" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A397" s="4"/>
       <c r="I397" s="6"/>
       <c r="J397" s="6"/>
@@ -28465,7 +28465,7 @@
       <c r="AI397" s="67"/>
       <c r="AJ397" s="40"/>
     </row>
-    <row r="398" spans="1:36" s="5" customFormat="1">
+    <row r="398" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A398" s="4"/>
       <c r="I398" s="6"/>
       <c r="J398" s="6"/>
@@ -28482,7 +28482,7 @@
       <c r="AI398" s="67"/>
       <c r="AJ398" s="40"/>
     </row>
-    <row r="399" spans="1:36" s="5" customFormat="1">
+    <row r="399" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A399" s="4"/>
       <c r="I399" s="6"/>
       <c r="J399" s="6"/>
@@ -28499,7 +28499,7 @@
       <c r="AI399" s="67"/>
       <c r="AJ399" s="40"/>
     </row>
-    <row r="400" spans="1:36" s="5" customFormat="1">
+    <row r="400" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A400" s="4"/>
       <c r="I400" s="6"/>
       <c r="J400" s="6"/>
@@ -28516,7 +28516,7 @@
       <c r="AI400" s="67"/>
       <c r="AJ400" s="40"/>
     </row>
-    <row r="401" spans="1:36" s="5" customFormat="1">
+    <row r="401" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A401" s="4"/>
       <c r="I401" s="6"/>
       <c r="J401" s="6"/>
@@ -28533,7 +28533,7 @@
       <c r="AI401" s="67"/>
       <c r="AJ401" s="40"/>
     </row>
-    <row r="402" spans="1:36" s="5" customFormat="1">
+    <row r="402" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A402" s="4"/>
       <c r="I402" s="6"/>
       <c r="J402" s="6"/>
@@ -28550,7 +28550,7 @@
       <c r="AI402" s="67"/>
       <c r="AJ402" s="40"/>
     </row>
-    <row r="403" spans="1:36" s="5" customFormat="1">
+    <row r="403" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A403" s="4"/>
       <c r="I403" s="6"/>
       <c r="J403" s="6"/>
@@ -28567,7 +28567,7 @@
       <c r="AI403" s="67"/>
       <c r="AJ403" s="40"/>
     </row>
-    <row r="404" spans="1:36" s="5" customFormat="1">
+    <row r="404" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A404" s="4"/>
       <c r="I404" s="6"/>
       <c r="J404" s="6"/>
@@ -28584,7 +28584,7 @@
       <c r="AI404" s="67"/>
       <c r="AJ404" s="40"/>
     </row>
-    <row r="405" spans="1:36" s="5" customFormat="1">
+    <row r="405" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A405" s="4"/>
       <c r="I405" s="6"/>
       <c r="J405" s="6"/>
@@ -28601,7 +28601,7 @@
       <c r="AI405" s="67"/>
       <c r="AJ405" s="40"/>
     </row>
-    <row r="406" spans="1:36" s="5" customFormat="1">
+    <row r="406" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A406" s="4"/>
       <c r="I406" s="6"/>
       <c r="J406" s="6"/>
@@ -28618,7 +28618,7 @@
       <c r="AI406" s="67"/>
       <c r="AJ406" s="40"/>
     </row>
-    <row r="407" spans="1:36" s="5" customFormat="1">
+    <row r="407" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A407" s="4"/>
       <c r="I407" s="6"/>
       <c r="J407" s="6"/>
@@ -28635,7 +28635,7 @@
       <c r="AI407" s="67"/>
       <c r="AJ407" s="40"/>
     </row>
-    <row r="408" spans="1:36" s="5" customFormat="1">
+    <row r="408" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A408" s="4"/>
       <c r="I408" s="6"/>
       <c r="J408" s="6"/>
@@ -28652,7 +28652,7 @@
       <c r="AI408" s="67"/>
       <c r="AJ408" s="40"/>
     </row>
-    <row r="409" spans="1:36" s="5" customFormat="1">
+    <row r="409" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A409" s="4"/>
       <c r="I409" s="6"/>
       <c r="J409" s="6"/>
@@ -28669,7 +28669,7 @@
       <c r="AI409" s="67"/>
       <c r="AJ409" s="40"/>
     </row>
-    <row r="410" spans="1:36" s="5" customFormat="1">
+    <row r="410" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A410" s="4"/>
       <c r="I410" s="6"/>
       <c r="J410" s="6"/>
@@ -28686,7 +28686,7 @@
       <c r="AI410" s="67"/>
       <c r="AJ410" s="40"/>
     </row>
-    <row r="411" spans="1:36" s="5" customFormat="1">
+    <row r="411" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A411" s="4"/>
       <c r="I411" s="6"/>
       <c r="J411" s="6"/>
@@ -28703,7 +28703,7 @@
       <c r="AI411" s="67"/>
       <c r="AJ411" s="40"/>
     </row>
-    <row r="412" spans="1:36" s="5" customFormat="1">
+    <row r="412" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A412" s="4"/>
       <c r="I412" s="6"/>
       <c r="J412" s="6"/>
@@ -28720,7 +28720,7 @@
       <c r="AI412" s="67"/>
       <c r="AJ412" s="40"/>
     </row>
-    <row r="413" spans="1:36" s="5" customFormat="1">
+    <row r="413" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A413" s="4"/>
       <c r="I413" s="6"/>
       <c r="J413" s="6"/>
@@ -28737,7 +28737,7 @@
       <c r="AI413" s="67"/>
       <c r="AJ413" s="40"/>
     </row>
-    <row r="414" spans="1:36" s="5" customFormat="1">
+    <row r="414" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A414" s="4"/>
       <c r="I414" s="6"/>
       <c r="J414" s="6"/>
@@ -28754,7 +28754,7 @@
       <c r="AI414" s="67"/>
       <c r="AJ414" s="40"/>
     </row>
-    <row r="415" spans="1:36" s="5" customFormat="1">
+    <row r="415" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A415" s="4"/>
       <c r="I415" s="6"/>
       <c r="J415" s="6"/>
@@ -28771,7 +28771,7 @@
       <c r="AI415" s="67"/>
       <c r="AJ415" s="40"/>
     </row>
-    <row r="416" spans="1:36" s="5" customFormat="1">
+    <row r="416" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A416" s="4"/>
       <c r="I416" s="6"/>
       <c r="J416" s="6"/>
@@ -28788,7 +28788,7 @@
       <c r="AI416" s="67"/>
       <c r="AJ416" s="40"/>
     </row>
-    <row r="417" spans="1:36" s="5" customFormat="1">
+    <row r="417" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A417" s="4"/>
       <c r="I417" s="6"/>
       <c r="J417" s="6"/>
@@ -28805,7 +28805,7 @@
       <c r="AI417" s="67"/>
       <c r="AJ417" s="40"/>
     </row>
-    <row r="418" spans="1:36" s="5" customFormat="1">
+    <row r="418" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A418" s="4"/>
       <c r="I418" s="6"/>
       <c r="J418" s="6"/>
@@ -28822,7 +28822,7 @@
       <c r="AI418" s="67"/>
       <c r="AJ418" s="40"/>
     </row>
-    <row r="419" spans="1:36" s="5" customFormat="1">
+    <row r="419" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A419" s="4"/>
       <c r="I419" s="6"/>
       <c r="J419" s="6"/>
@@ -28839,7 +28839,7 @@
       <c r="AI419" s="67"/>
       <c r="AJ419" s="40"/>
     </row>
-    <row r="420" spans="1:36" s="5" customFormat="1">
+    <row r="420" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A420" s="4"/>
       <c r="I420" s="6"/>
       <c r="J420" s="6"/>
@@ -28856,7 +28856,7 @@
       <c r="AI420" s="67"/>
       <c r="AJ420" s="40"/>
     </row>
-    <row r="421" spans="1:36" s="5" customFormat="1">
+    <row r="421" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A421" s="4"/>
       <c r="I421" s="6"/>
       <c r="J421" s="6"/>
@@ -28873,7 +28873,7 @@
       <c r="AI421" s="67"/>
       <c r="AJ421" s="40"/>
     </row>
-    <row r="422" spans="1:36" s="5" customFormat="1">
+    <row r="422" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A422" s="4"/>
       <c r="I422" s="6"/>
       <c r="J422" s="6"/>
@@ -28890,7 +28890,7 @@
       <c r="AI422" s="67"/>
       <c r="AJ422" s="40"/>
     </row>
-    <row r="423" spans="1:36" s="5" customFormat="1">
+    <row r="423" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A423" s="4"/>
       <c r="I423" s="6"/>
       <c r="J423" s="6"/>
@@ -28907,7 +28907,7 @@
       <c r="AI423" s="67"/>
       <c r="AJ423" s="40"/>
     </row>
-    <row r="424" spans="1:36" s="5" customFormat="1">
+    <row r="424" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A424" s="4"/>
       <c r="I424" s="6"/>
       <c r="J424" s="6"/>
@@ -28924,7 +28924,7 @@
       <c r="AI424" s="67"/>
       <c r="AJ424" s="40"/>
     </row>
-    <row r="425" spans="1:36" s="5" customFormat="1">
+    <row r="425" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A425" s="4"/>
       <c r="I425" s="6"/>
       <c r="J425" s="6"/>
@@ -28941,7 +28941,7 @@
       <c r="AI425" s="67"/>
       <c r="AJ425" s="40"/>
     </row>
-    <row r="426" spans="1:36" s="5" customFormat="1">
+    <row r="426" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A426" s="4"/>
       <c r="I426" s="6"/>
       <c r="J426" s="6"/>
@@ -28958,7 +28958,7 @@
       <c r="AI426" s="67"/>
       <c r="AJ426" s="40"/>
     </row>
-    <row r="427" spans="1:36" s="5" customFormat="1">
+    <row r="427" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A427" s="4"/>
       <c r="I427" s="6"/>
       <c r="J427" s="6"/>
@@ -28975,7 +28975,7 @@
       <c r="AI427" s="67"/>
       <c r="AJ427" s="40"/>
     </row>
-    <row r="428" spans="1:36" s="5" customFormat="1">
+    <row r="428" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A428" s="4"/>
       <c r="I428" s="6"/>
       <c r="J428" s="6"/>
@@ -28992,7 +28992,7 @@
       <c r="AI428" s="67"/>
       <c r="AJ428" s="40"/>
     </row>
-    <row r="429" spans="1:36" s="5" customFormat="1">
+    <row r="429" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A429" s="4"/>
       <c r="I429" s="6"/>
       <c r="J429" s="6"/>
@@ -29009,7 +29009,7 @@
       <c r="AI429" s="67"/>
       <c r="AJ429" s="40"/>
     </row>
-    <row r="430" spans="1:36" s="5" customFormat="1">
+    <row r="430" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A430" s="4"/>
       <c r="I430" s="6"/>
       <c r="J430" s="6"/>
@@ -29026,7 +29026,7 @@
       <c r="AI430" s="67"/>
       <c r="AJ430" s="40"/>
     </row>
-    <row r="431" spans="1:36" s="5" customFormat="1">
+    <row r="431" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A431" s="4"/>
       <c r="I431" s="6"/>
       <c r="J431" s="6"/>
@@ -29043,7 +29043,7 @@
       <c r="AI431" s="67"/>
       <c r="AJ431" s="40"/>
     </row>
-    <row r="432" spans="1:36" s="5" customFormat="1" ht="12.75" customHeight="1">
+    <row r="432" spans="1:36" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A432" s="4"/>
       <c r="I432" s="6"/>
       <c r="J432" s="6"/>
@@ -29060,7 +29060,7 @@
       <c r="AI432" s="67"/>
       <c r="AJ432" s="40"/>
     </row>
-    <row r="433" spans="1:36" s="5" customFormat="1">
+    <row r="433" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A433" s="4"/>
       <c r="I433" s="6"/>
       <c r="J433" s="6"/>
@@ -29077,7 +29077,7 @@
       <c r="AI433" s="67"/>
       <c r="AJ433" s="40"/>
     </row>
-    <row r="434" spans="1:36" s="5" customFormat="1">
+    <row r="434" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A434" s="4"/>
       <c r="I434" s="6"/>
       <c r="J434" s="6"/>
@@ -29094,7 +29094,7 @@
       <c r="AI434" s="67"/>
       <c r="AJ434" s="40"/>
     </row>
-    <row r="435" spans="1:36" s="5" customFormat="1">
+    <row r="435" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A435" s="4"/>
       <c r="I435" s="6"/>
       <c r="J435" s="6"/>
@@ -29111,7 +29111,7 @@
       <c r="AI435" s="67"/>
       <c r="AJ435" s="40"/>
     </row>
-    <row r="436" spans="1:36" s="5" customFormat="1">
+    <row r="436" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A436" s="4"/>
       <c r="I436" s="6"/>
       <c r="J436" s="6"/>
@@ -29128,7 +29128,7 @@
       <c r="AI436" s="67"/>
       <c r="AJ436" s="40"/>
     </row>
-    <row r="437" spans="1:36" s="5" customFormat="1">
+    <row r="437" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A437" s="4"/>
       <c r="I437" s="6"/>
       <c r="J437" s="6"/>
@@ -29145,7 +29145,7 @@
       <c r="AI437" s="67"/>
       <c r="AJ437" s="40"/>
     </row>
-    <row r="438" spans="1:36" s="5" customFormat="1">
+    <row r="438" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A438" s="4"/>
       <c r="I438" s="6"/>
       <c r="J438" s="6"/>
@@ -29162,7 +29162,7 @@
       <c r="AI438" s="67"/>
       <c r="AJ438" s="40"/>
     </row>
-    <row r="439" spans="1:36" s="5" customFormat="1">
+    <row r="439" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A439" s="4"/>
       <c r="I439" s="6"/>
       <c r="J439" s="6"/>
@@ -29179,7 +29179,7 @@
       <c r="AI439" s="67"/>
       <c r="AJ439" s="40"/>
     </row>
-    <row r="440" spans="1:36" s="5" customFormat="1">
+    <row r="440" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A440" s="4"/>
       <c r="I440" s="6"/>
       <c r="J440" s="6"/>
@@ -29196,7 +29196,7 @@
       <c r="AI440" s="67"/>
       <c r="AJ440" s="40"/>
     </row>
-    <row r="441" spans="1:36" s="5" customFormat="1">
+    <row r="441" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A441" s="4"/>
       <c r="I441" s="6"/>
       <c r="J441" s="6"/>
@@ -29213,7 +29213,7 @@
       <c r="AI441" s="67"/>
       <c r="AJ441" s="40"/>
     </row>
-    <row r="442" spans="1:36" s="5" customFormat="1">
+    <row r="442" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A442" s="4"/>
       <c r="I442" s="6"/>
       <c r="J442" s="6"/>
@@ -29230,7 +29230,7 @@
       <c r="AI442" s="67"/>
       <c r="AJ442" s="40"/>
     </row>
-    <row r="443" spans="1:36" s="5" customFormat="1">
+    <row r="443" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A443" s="4"/>
       <c r="I443" s="6"/>
       <c r="J443" s="6"/>
@@ -29247,7 +29247,7 @@
       <c r="AI443" s="67"/>
       <c r="AJ443" s="40"/>
     </row>
-    <row r="444" spans="1:36" s="5" customFormat="1">
+    <row r="444" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A444" s="4"/>
       <c r="I444" s="6"/>
       <c r="J444" s="6"/>
@@ -29264,7 +29264,7 @@
       <c r="AI444" s="67"/>
       <c r="AJ444" s="40"/>
     </row>
-    <row r="445" spans="1:36" s="5" customFormat="1">
+    <row r="445" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A445" s="4"/>
       <c r="I445" s="6"/>
       <c r="J445" s="6"/>
@@ -29281,7 +29281,7 @@
       <c r="AI445" s="67"/>
       <c r="AJ445" s="40"/>
     </row>
-    <row r="446" spans="1:36" s="5" customFormat="1">
+    <row r="446" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A446" s="4"/>
       <c r="I446" s="6"/>
       <c r="J446" s="6"/>
@@ -29298,7 +29298,7 @@
       <c r="AI446" s="67"/>
       <c r="AJ446" s="40"/>
     </row>
-    <row r="447" spans="1:36" s="5" customFormat="1">
+    <row r="447" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A447" s="4"/>
       <c r="I447" s="6"/>
       <c r="J447" s="6"/>
@@ -29315,7 +29315,7 @@
       <c r="AI447" s="67"/>
       <c r="AJ447" s="40"/>
     </row>
-    <row r="448" spans="1:36" s="5" customFormat="1">
+    <row r="448" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A448" s="4"/>
       <c r="I448" s="6"/>
       <c r="J448" s="6"/>

</xml_diff>